<commit_message>
generated from ./SC24/HVCB.json at 4381d6c
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
   <si>
     <t>ID</t>
   </si>
@@ -2801,9 +2801,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29117,7 +29114,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>928</v>
+        <v>863</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29176,7 +29173,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29235,7 +29232,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29294,7 +29291,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29353,7 +29350,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29412,7 +29409,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29439,10 +29436,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="I457" s="6" t="s">
         <v>934</v>
-      </c>
-      <c r="I457" s="6" t="s">
-        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29469,18 +29466,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="U457" s="6" t="s">
         <v>936</v>
-      </c>
-      <c r="U457" s="6" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B458" s="2" t="s">
         <v>938</v>
-      </c>
-      <c r="B458" s="2" t="s">
-        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29498,10 +29495,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="I458" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="I458" s="2" t="s">
-        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29528,16 +29525,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="B459" s="5" t="s">
         <v>938</v>
-      </c>
-      <c r="B459" s="5" t="s">
-        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29555,10 +29552,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29585,22 +29582,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="C460" s="2">
+        <v>0</v>
+      </c>
+      <c r="D460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="C460" s="2">
-        <v>0</v>
-      </c>
-      <c r="D460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29626,16 +29623,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B461" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B461" s="2" t="s">
+      <c r="C461" s="2">
+        <v>0</v>
+      </c>
+      <c r="D461" s="2" t="s">
         <v>948</v>
-      </c>
-      <c r="C461" s="2">
-        <v>0</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29661,10 +29658,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="B462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29682,7 +29679,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29710,16 +29707,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B463" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B463" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29737,7 +29734,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29761,16 +29758,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B464" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B464" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29788,7 +29785,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29812,16 +29809,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29839,7 +29836,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29863,16 +29860,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29890,7 +29887,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29914,16 +29911,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29941,7 +29938,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29967,16 +29964,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29994,7 +29991,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30020,18 +30017,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="U468" s="6" t="s">
         <v>961</v>
-      </c>
-      <c r="U468" s="6" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B469" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30049,7 +30046,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30077,16 +30074,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30104,7 +30101,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30128,16 +30125,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B471" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B471" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30155,7 +30152,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30179,16 +30176,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30206,7 +30203,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30230,16 +30227,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30257,7 +30254,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30281,16 +30278,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30308,7 +30305,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30334,16 +30331,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30361,7 +30358,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30387,18 +30384,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B476" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30416,7 +30413,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30444,16 +30441,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30471,7 +30468,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30495,16 +30492,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B478" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30522,7 +30519,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30546,16 +30543,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30573,7 +30570,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30597,16 +30594,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30624,7 +30621,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30648,16 +30645,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30675,7 +30672,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30701,16 +30698,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30728,7 +30725,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30754,18 +30751,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B483" s="2" t="s">
         <v>984</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30783,7 +30780,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30811,16 +30808,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30838,7 +30835,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30862,16 +30859,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B485" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B485" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30889,7 +30886,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30913,16 +30910,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30940,7 +30937,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30964,16 +30961,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30991,7 +30988,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31015,16 +31012,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31042,7 +31039,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31068,16 +31065,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31095,7 +31092,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31121,18 +31118,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B490" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31150,7 +31147,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31178,16 +31175,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31205,7 +31202,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31229,16 +31226,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B492" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B492" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31256,7 +31253,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31280,16 +31277,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31307,7 +31304,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31331,16 +31328,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31358,7 +31355,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31382,16 +31379,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31409,7 +31406,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31435,16 +31432,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31462,7 +31459,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31488,18 +31485,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B497" s="2" t="s">
         <v>1005</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31517,7 +31514,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31545,16 +31542,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31572,7 +31569,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31596,16 +31593,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B499" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B499" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31623,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31647,16 +31644,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31674,7 +31671,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31698,16 +31695,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31725,7 +31722,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31749,16 +31746,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31776,7 +31773,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31802,16 +31799,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31829,7 +31826,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31855,18 +31852,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B504" s="2" t="s">
         <v>1016</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31884,7 +31881,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31912,16 +31909,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31939,7 +31936,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31963,16 +31960,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B506" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B506" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31990,7 +31987,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32014,16 +32011,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32041,7 +32038,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32065,16 +32062,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32092,7 +32089,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32116,16 +32113,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32143,7 +32140,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32169,16 +32166,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32196,7 +32193,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32222,18 +32219,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="U510" s="6" t="s">
         <v>1026</v>
-      </c>
-      <c r="U510" s="6" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B511" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="B511" s="2" t="s">
-        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32251,7 +32248,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32279,16 +32276,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32306,7 +32303,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32330,16 +32327,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B513" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B513" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32357,7 +32354,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32381,16 +32378,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32408,7 +32405,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32432,16 +32429,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32459,7 +32456,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32483,16 +32480,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32510,7 +32507,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32536,16 +32533,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32563,7 +32560,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32589,10 +32586,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at 208ba34
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
   <si>
     <t>ID</t>
   </si>
@@ -2801,6 +2801,9 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29114,7 +29117,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>863</v>
+        <v>928</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29173,7 +29176,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29232,7 +29235,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29291,7 +29294,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29350,7 +29353,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29409,7 +29412,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29436,10 +29439,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I457" s="6" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29466,18 +29469,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U457" s="6" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29495,10 +29498,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="I458" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29525,16 +29528,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29552,10 +29555,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29582,22 +29585,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C460" s="2">
         <v>0</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29623,16 +29626,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C461" s="2">
         <v>0</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29658,10 +29661,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29679,7 +29682,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29707,16 +29710,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29734,7 +29737,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29758,16 +29761,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29785,7 +29788,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29809,16 +29812,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29836,7 +29839,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29860,16 +29863,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29887,7 +29890,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29911,16 +29914,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29938,7 +29941,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29964,16 +29967,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29991,7 +29994,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30017,18 +30020,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U468" s="6" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30046,7 +30049,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30074,16 +30077,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30101,7 +30104,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30125,16 +30128,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30152,7 +30155,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30176,16 +30179,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30203,7 +30206,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30227,16 +30230,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30254,7 +30257,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30278,16 +30281,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30305,7 +30308,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30331,16 +30334,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30358,7 +30361,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30384,18 +30387,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30413,7 +30416,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30441,16 +30444,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30468,7 +30471,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30492,16 +30495,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30519,7 +30522,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30543,16 +30546,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30570,7 +30573,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30594,16 +30597,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30621,7 +30624,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30645,16 +30648,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30672,7 +30675,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30698,16 +30701,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30725,7 +30728,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30751,18 +30754,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30780,7 +30783,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30808,16 +30811,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30835,7 +30838,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30859,16 +30862,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30886,7 +30889,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30910,16 +30913,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30937,7 +30940,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30961,16 +30964,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30988,7 +30991,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31012,16 +31015,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31039,7 +31042,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31065,16 +31068,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31092,7 +31095,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31118,18 +31121,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31147,7 +31150,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31175,16 +31178,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31202,7 +31205,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31226,16 +31229,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31253,7 +31256,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31277,16 +31280,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31304,7 +31307,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31328,16 +31331,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31355,7 +31358,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31379,16 +31382,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31406,7 +31409,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31432,16 +31435,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31459,7 +31462,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31485,18 +31488,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31514,7 +31517,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31542,16 +31545,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31569,7 +31572,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31593,16 +31596,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31620,7 +31623,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31644,16 +31647,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31671,7 +31674,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31695,16 +31698,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31722,7 +31725,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31746,16 +31749,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31773,7 +31776,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31799,16 +31802,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31826,7 +31829,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31852,18 +31855,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31881,7 +31884,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31909,16 +31912,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31936,7 +31939,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31960,16 +31963,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31987,7 +31990,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32011,16 +32014,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32038,7 +32041,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32062,16 +32065,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32089,7 +32092,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32113,16 +32116,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32140,7 +32143,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32166,16 +32169,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32193,7 +32196,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32219,18 +32222,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="U510" s="6" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32248,7 +32251,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32276,16 +32279,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32303,7 +32306,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32327,16 +32330,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32354,7 +32357,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32378,16 +32381,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32405,7 +32408,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32429,16 +32432,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32456,7 +32459,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32480,16 +32483,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32507,7 +32510,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32533,16 +32536,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32560,7 +32563,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32586,10 +32589,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at e58882b
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
   <si>
     <t>ID</t>
   </si>
@@ -2801,9 +2801,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29117,7 +29114,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>928</v>
+        <v>863</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29176,7 +29173,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29235,7 +29232,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29294,7 +29291,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29353,7 +29350,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29412,7 +29409,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29439,10 +29436,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="I457" s="6" t="s">
         <v>934</v>
-      </c>
-      <c r="I457" s="6" t="s">
-        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29469,18 +29466,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="U457" s="6" t="s">
         <v>936</v>
-      </c>
-      <c r="U457" s="6" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B458" s="2" t="s">
         <v>938</v>
-      </c>
-      <c r="B458" s="2" t="s">
-        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29498,10 +29495,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="I458" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="I458" s="2" t="s">
-        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29528,16 +29525,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="B459" s="5" t="s">
         <v>938</v>
-      </c>
-      <c r="B459" s="5" t="s">
-        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29555,10 +29552,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29585,22 +29582,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="C460" s="2">
+        <v>0</v>
+      </c>
+      <c r="D460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="C460" s="2">
-        <v>0</v>
-      </c>
-      <c r="D460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29626,16 +29623,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B461" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B461" s="2" t="s">
+      <c r="C461" s="2">
+        <v>0</v>
+      </c>
+      <c r="D461" s="2" t="s">
         <v>948</v>
-      </c>
-      <c r="C461" s="2">
-        <v>0</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29661,10 +29658,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="B462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29682,7 +29679,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29710,16 +29707,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B463" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B463" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29737,7 +29734,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29761,16 +29758,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B464" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B464" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29788,7 +29785,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29812,16 +29809,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29839,7 +29836,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29863,16 +29860,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29890,7 +29887,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29914,16 +29911,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29941,7 +29938,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29967,16 +29964,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29994,7 +29991,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30020,18 +30017,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="U468" s="6" t="s">
         <v>961</v>
-      </c>
-      <c r="U468" s="6" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B469" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30049,7 +30046,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30077,16 +30074,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30104,7 +30101,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30128,16 +30125,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B471" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B471" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30155,7 +30152,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30179,16 +30176,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30206,7 +30203,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30230,16 +30227,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30257,7 +30254,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30281,16 +30278,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30308,7 +30305,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30334,16 +30331,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30361,7 +30358,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30387,18 +30384,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B476" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30416,7 +30413,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30444,16 +30441,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30471,7 +30468,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30495,16 +30492,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B478" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30522,7 +30519,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30546,16 +30543,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30573,7 +30570,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30597,16 +30594,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30624,7 +30621,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30648,16 +30645,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30675,7 +30672,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30701,16 +30698,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30728,7 +30725,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30754,18 +30751,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B483" s="2" t="s">
         <v>984</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30783,7 +30780,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30811,16 +30808,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30838,7 +30835,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30862,16 +30859,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B485" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B485" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30889,7 +30886,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30913,16 +30910,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30940,7 +30937,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30964,16 +30961,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30991,7 +30988,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31015,16 +31012,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31042,7 +31039,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31068,16 +31065,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31095,7 +31092,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31121,18 +31118,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B490" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31150,7 +31147,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31178,16 +31175,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31205,7 +31202,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31229,16 +31226,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B492" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B492" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31256,7 +31253,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31280,16 +31277,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31307,7 +31304,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31331,16 +31328,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31358,7 +31355,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31382,16 +31379,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31409,7 +31406,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31435,16 +31432,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31462,7 +31459,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31488,18 +31485,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B497" s="2" t="s">
         <v>1005</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31517,7 +31514,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31545,16 +31542,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31572,7 +31569,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31596,16 +31593,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B499" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B499" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31623,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31647,16 +31644,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31674,7 +31671,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31698,16 +31695,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31725,7 +31722,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31749,16 +31746,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31776,7 +31773,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31802,16 +31799,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31829,7 +31826,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31855,18 +31852,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B504" s="2" t="s">
         <v>1016</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31884,7 +31881,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31912,16 +31909,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31939,7 +31936,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31963,16 +31960,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B506" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B506" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31990,7 +31987,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32014,16 +32011,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32041,7 +32038,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32065,16 +32062,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32092,7 +32089,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32116,16 +32113,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32143,7 +32140,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32169,16 +32166,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32196,7 +32193,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32222,18 +32219,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="U510" s="6" t="s">
         <v>1026</v>
-      </c>
-      <c r="U510" s="6" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B511" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="B511" s="2" t="s">
-        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32251,7 +32248,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32279,16 +32276,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32306,7 +32303,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32330,16 +32327,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B513" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B513" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32357,7 +32354,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32381,16 +32378,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32408,7 +32405,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32432,16 +32429,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32459,7 +32456,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32483,16 +32480,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32510,7 +32507,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32536,16 +32533,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32563,7 +32560,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32589,10 +32586,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at fb473e1
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
   <si>
     <t>ID</t>
   </si>
@@ -2801,6 +2801,9 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29114,7 +29117,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>863</v>
+        <v>928</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29173,7 +29176,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29232,7 +29235,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29291,7 +29294,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29350,7 +29353,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29409,7 +29412,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29436,10 +29439,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I457" s="6" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29466,18 +29469,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U457" s="6" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29495,10 +29498,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="I458" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29525,16 +29528,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29552,10 +29555,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29582,22 +29585,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C460" s="2">
         <v>0</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29623,16 +29626,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C461" s="2">
         <v>0</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29658,10 +29661,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29679,7 +29682,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29707,16 +29710,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29734,7 +29737,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29758,16 +29761,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29785,7 +29788,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29809,16 +29812,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29836,7 +29839,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29860,16 +29863,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29887,7 +29890,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29911,16 +29914,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29938,7 +29941,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29964,16 +29967,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29991,7 +29994,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30017,18 +30020,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U468" s="6" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30046,7 +30049,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30074,16 +30077,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30101,7 +30104,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30125,16 +30128,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30152,7 +30155,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30176,16 +30179,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30203,7 +30206,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30227,16 +30230,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30254,7 +30257,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30278,16 +30281,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30305,7 +30308,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30331,16 +30334,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30358,7 +30361,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30384,18 +30387,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30413,7 +30416,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30441,16 +30444,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30468,7 +30471,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30492,16 +30495,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30519,7 +30522,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30543,16 +30546,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30570,7 +30573,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30594,16 +30597,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30621,7 +30624,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30645,16 +30648,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30672,7 +30675,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30698,16 +30701,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30725,7 +30728,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30751,18 +30754,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30780,7 +30783,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30808,16 +30811,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30835,7 +30838,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30859,16 +30862,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30886,7 +30889,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30910,16 +30913,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30937,7 +30940,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30961,16 +30964,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30988,7 +30991,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31012,16 +31015,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31039,7 +31042,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31065,16 +31068,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31092,7 +31095,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31118,18 +31121,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31147,7 +31150,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31175,16 +31178,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31202,7 +31205,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31226,16 +31229,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31253,7 +31256,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31277,16 +31280,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31304,7 +31307,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31328,16 +31331,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31355,7 +31358,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31379,16 +31382,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31406,7 +31409,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31432,16 +31435,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31459,7 +31462,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31485,18 +31488,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31514,7 +31517,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31542,16 +31545,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31569,7 +31572,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31593,16 +31596,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31620,7 +31623,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31644,16 +31647,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31671,7 +31674,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31695,16 +31698,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31722,7 +31725,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31746,16 +31749,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31773,7 +31776,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31799,16 +31802,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31826,7 +31829,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31852,18 +31855,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31881,7 +31884,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31909,16 +31912,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31936,7 +31939,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31960,16 +31963,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31987,7 +31990,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32011,16 +32014,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32038,7 +32041,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32062,16 +32065,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32089,7 +32092,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32113,16 +32116,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32140,7 +32143,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32166,16 +32169,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32193,7 +32196,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32219,18 +32222,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="U510" s="6" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32248,7 +32251,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32276,16 +32279,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32303,7 +32306,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32327,16 +32330,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32354,7 +32357,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32378,16 +32381,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32405,7 +32408,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32429,16 +32432,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32456,7 +32459,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32480,16 +32483,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32507,7 +32510,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32533,16 +32536,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32560,7 +32563,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32586,10 +32589,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at e2baa35
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
   <si>
     <t>ID</t>
   </si>
@@ -2801,9 +2801,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29117,7 +29114,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>928</v>
+        <v>863</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29176,7 +29173,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29235,7 +29232,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29294,7 +29291,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29353,7 +29350,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29412,7 +29409,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29439,10 +29436,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
+        <v>933</v>
+      </c>
+      <c r="I457" s="6" t="s">
         <v>934</v>
-      </c>
-      <c r="I457" s="6" t="s">
-        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29469,18 +29466,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
+        <v>935</v>
+      </c>
+      <c r="U457" s="6" t="s">
         <v>936</v>
-      </c>
-      <c r="U457" s="6" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="B458" s="2" t="s">
         <v>938</v>
-      </c>
-      <c r="B458" s="2" t="s">
-        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29498,10 +29495,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
+        <v>939</v>
+      </c>
+      <c r="I458" s="2" t="s">
         <v>940</v>
-      </c>
-      <c r="I458" s="2" t="s">
-        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29528,16 +29525,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="B459" s="5" t="s">
         <v>938</v>
-      </c>
-      <c r="B459" s="5" t="s">
-        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29555,10 +29552,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29585,22 +29582,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="C460" s="2">
+        <v>0</v>
+      </c>
+      <c r="D460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="C460" s="2">
-        <v>0</v>
-      </c>
-      <c r="D460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29626,16 +29623,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
+        <v>946</v>
+      </c>
+      <c r="B461" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B461" s="2" t="s">
+      <c r="C461" s="2">
+        <v>0</v>
+      </c>
+      <c r="D461" s="2" t="s">
         <v>948</v>
-      </c>
-      <c r="C461" s="2">
-        <v>0</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29661,10 +29658,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>949</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="B462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29682,7 +29679,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29710,16 +29707,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B463" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B463" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29737,7 +29734,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29761,16 +29758,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B464" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B464" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29788,7 +29785,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29812,16 +29809,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29839,7 +29836,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29863,16 +29860,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29890,7 +29887,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29914,16 +29911,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29941,7 +29938,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29967,16 +29964,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>950</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29994,7 +29991,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30020,18 +30017,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="U468" s="6" t="s">
         <v>961</v>
-      </c>
-      <c r="U468" s="6" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B469" s="2" t="s">
         <v>963</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30049,7 +30046,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30077,16 +30074,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30104,7 +30101,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30128,16 +30125,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B471" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B471" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30155,7 +30152,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30179,16 +30176,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30206,7 +30203,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30230,16 +30227,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30257,7 +30254,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30281,16 +30278,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30308,7 +30305,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30334,16 +30331,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>962</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>963</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30361,7 +30358,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30387,18 +30384,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="B476" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30416,7 +30413,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30444,16 +30441,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30471,7 +30468,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30495,16 +30492,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B478" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30522,7 +30519,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30546,16 +30543,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30573,7 +30570,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30597,16 +30594,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30624,7 +30621,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30648,16 +30645,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30675,7 +30672,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30701,16 +30698,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>974</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30728,7 +30725,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30754,18 +30751,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
+        <v>983</v>
+      </c>
+      <c r="B483" s="2" t="s">
         <v>984</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30783,7 +30780,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30811,16 +30808,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30838,7 +30835,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30862,16 +30859,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B485" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B485" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30889,7 +30886,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30913,16 +30910,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30940,7 +30937,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30964,16 +30961,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30991,7 +30988,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31015,16 +31012,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31042,7 +31039,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31068,16 +31065,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>983</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>984</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31095,7 +31092,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31121,18 +31118,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="B490" s="2" t="s">
         <v>994</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31150,7 +31147,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31178,16 +31175,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31205,7 +31202,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31229,16 +31226,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B492" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B492" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31256,7 +31253,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31280,16 +31277,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31307,7 +31304,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31331,16 +31328,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31358,7 +31355,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31382,16 +31379,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31409,7 +31406,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31435,16 +31432,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>993</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31462,7 +31459,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31488,18 +31485,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B497" s="2" t="s">
         <v>1005</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31517,7 +31514,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31545,16 +31542,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31572,7 +31569,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31596,16 +31593,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B499" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B499" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31623,7 +31620,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31647,16 +31644,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31674,7 +31671,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31698,16 +31695,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31725,7 +31722,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31749,16 +31746,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31776,7 +31773,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31802,16 +31799,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1005</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31829,7 +31826,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31855,18 +31852,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B504" s="2" t="s">
         <v>1016</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31884,7 +31881,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31912,16 +31909,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31939,7 +31936,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31963,16 +31960,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B506" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B506" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31990,7 +31987,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32014,16 +32011,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32041,7 +32038,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32065,16 +32062,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32092,7 +32089,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32116,16 +32113,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32143,7 +32140,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32169,16 +32166,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1016</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32196,7 +32193,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32222,18 +32219,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="U510" s="6" t="s">
         <v>1026</v>
-      </c>
-      <c r="U510" s="6" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B511" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="B511" s="2" t="s">
-        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32251,7 +32248,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32279,16 +32276,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32306,7 +32303,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32330,16 +32327,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B513" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B513" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32357,7 +32354,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32381,16 +32378,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32408,7 +32405,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32432,16 +32429,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32459,7 +32456,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32483,16 +32480,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32510,7 +32507,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32536,16 +32533,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1028</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32563,7 +32560,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32589,10 +32586,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at 2494425
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
   <si>
     <t>ID</t>
   </si>
@@ -2801,6 +2801,9 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29114,7 +29117,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>863</v>
+        <v>928</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29173,7 +29176,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29232,7 +29235,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29291,7 +29294,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29350,7 +29353,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29409,7 +29412,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29436,10 +29439,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I457" s="6" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29466,18 +29469,18 @@
       <c r="R457" s="8"/>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U457" s="6" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29495,10 +29498,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="I458" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29525,16 +29528,16 @@
       <c r="R458" s="4"/>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29552,10 +29555,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29582,22 +29585,22 @@
       <c r="R459" s="8"/>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C460" s="2">
         <v>0</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29623,16 +29626,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C461" s="2">
         <v>0</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29658,10 +29661,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29679,7 +29682,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29707,16 +29710,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29734,7 +29737,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29758,16 +29761,16 @@
       </c>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29785,7 +29788,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29809,16 +29812,16 @@
       </c>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29836,7 +29839,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29860,16 +29863,16 @@
       </c>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29887,7 +29890,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29911,16 +29914,16 @@
       </c>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29938,7 +29941,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29964,16 +29967,16 @@
       </c>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29991,7 +29994,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30017,18 +30020,18 @@
       </c>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U468" s="6" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30046,7 +30049,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30074,16 +30077,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30101,7 +30104,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30125,16 +30128,16 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30152,7 +30155,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30176,16 +30179,16 @@
       </c>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30203,7 +30206,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30227,16 +30230,16 @@
       </c>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30254,7 +30257,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30278,16 +30281,16 @@
       </c>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30305,7 +30308,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30331,16 +30334,16 @@
       </c>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30358,7 +30361,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30384,18 +30387,18 @@
       </c>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30413,7 +30416,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30441,16 +30444,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30468,7 +30471,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30492,16 +30495,16 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30519,7 +30522,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30543,16 +30546,16 @@
       </c>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30570,7 +30573,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30594,16 +30597,16 @@
       </c>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30621,7 +30624,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30645,16 +30648,16 @@
       </c>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30672,7 +30675,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30698,16 +30701,16 @@
       </c>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30725,7 +30728,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30751,18 +30754,18 @@
       </c>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30780,7 +30783,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30808,16 +30811,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30835,7 +30838,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30859,16 +30862,16 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30886,7 +30889,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30910,16 +30913,16 @@
       </c>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30937,7 +30940,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30961,16 +30964,16 @@
       </c>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30988,7 +30991,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31012,16 +31015,16 @@
       </c>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31039,7 +31042,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31065,16 +31068,16 @@
       </c>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31092,7 +31095,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31118,18 +31121,18 @@
       </c>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31147,7 +31150,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31175,16 +31178,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31202,7 +31205,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31226,16 +31229,16 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31253,7 +31256,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31277,16 +31280,16 @@
       </c>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31304,7 +31307,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31328,16 +31331,16 @@
       </c>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31355,7 +31358,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31379,16 +31382,16 @@
       </c>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31406,7 +31409,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31432,16 +31435,16 @@
       </c>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31459,7 +31462,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31485,18 +31488,18 @@
       </c>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31514,7 +31517,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31542,16 +31545,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31569,7 +31572,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31593,16 +31596,16 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31620,7 +31623,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31644,16 +31647,16 @@
       </c>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31671,7 +31674,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31695,16 +31698,16 @@
       </c>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31722,7 +31725,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31746,16 +31749,16 @@
       </c>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31773,7 +31776,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31799,16 +31802,16 @@
       </c>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31826,7 +31829,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31852,18 +31855,18 @@
       </c>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31881,7 +31884,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31909,16 +31912,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31936,7 +31939,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31960,16 +31963,16 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31987,7 +31990,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32011,16 +32014,16 @@
       </c>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32038,7 +32041,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32062,16 +32065,16 @@
       </c>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32089,7 +32092,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32113,16 +32116,16 @@
       </c>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32140,7 +32143,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32166,16 +32169,16 @@
       </c>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32193,7 +32196,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32219,18 +32222,18 @@
       </c>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="U510" s="6" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32248,7 +32251,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32276,16 +32279,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32303,7 +32306,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32327,16 +32330,16 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32354,7 +32357,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32378,16 +32381,16 @@
       </c>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32405,7 +32408,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32429,16 +32432,16 @@
       </c>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32456,7 +32459,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32480,16 +32483,16 @@
       </c>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32507,7 +32510,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32533,16 +32536,16 @@
       </c>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32560,7 +32563,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32586,10 +32589,10 @@
       </c>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at 67d5e61
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1039">
   <si>
     <t>ID</t>
   </si>
@@ -2801,6 +2801,9 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29121,7 +29124,7 @@
         <v>0</v>
       </c>
       <c r="T451" s="2" t="s">
-        <v>863</v>
+        <v>928</v>
       </c>
       <c r="U451" s="2"/>
     </row>
@@ -29180,7 +29183,7 @@
         <v>1</v>
       </c>
       <c r="T452" s="6" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="U452" s="5"/>
     </row>
@@ -29239,7 +29242,7 @@
         <v>2</v>
       </c>
       <c r="T453" s="6" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="U453" s="5"/>
     </row>
@@ -29298,7 +29301,7 @@
         <v>3</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29357,7 +29360,7 @@
         <v>4</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29416,7 +29419,7 @@
         <v>6</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29443,10 +29446,10 @@
         <v>0</v>
       </c>
       <c r="H457" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="I457" s="6" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="J457" s="6">
         <v>16</v>
@@ -29473,18 +29476,18 @@
       </c>
       <c r="S457" s="6"/>
       <c r="T457" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U457" s="6" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="458" spans="1:21">
       <c r="A458" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C458" s="2">
         <v>1000</v>
@@ -29502,10 +29505,10 @@
         <v>0</v>
       </c>
       <c r="H458" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="I458" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J458" s="2">
         <v>32</v>
@@ -29532,16 +29535,16 @@
       </c>
       <c r="S458" s="2"/>
       <c r="T458" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U458" s="2"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C459" s="5">
         <v>1000</v>
@@ -29559,10 +29562,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="J459" s="6">
         <v>32</v>
@@ -29589,22 +29592,22 @@
       </c>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C460" s="2">
         <v>0</v>
       </c>
       <c r="D460" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E460" s="2" t="s">
         <v>24</v>
@@ -29630,16 +29633,16 @@
     </row>
     <row r="461" spans="1:21">
       <c r="A461" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C461" s="2">
         <v>0</v>
       </c>
       <c r="D461" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E461" s="2" t="s">
         <v>24</v>
@@ -29665,10 +29668,10 @@
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C462" s="2">
         <v>20</v>
@@ -29686,7 +29689,7 @@
         <v>0</v>
       </c>
       <c r="H462" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="I462" s="2"/>
       <c r="J462" s="2">
@@ -29714,16 +29717,16 @@
         <v>0</v>
       </c>
       <c r="T462" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="U462" s="2"/>
     </row>
     <row r="463" spans="1:21" outlineLevel="1">
       <c r="A463" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B463" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C463" s="5">
         <v>20</v>
@@ -29741,7 +29744,7 @@
         <v>0</v>
       </c>
       <c r="H463" s="6" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="I463" s="6"/>
       <c r="J463" s="6">
@@ -29765,16 +29768,16 @@
       <c r="R463" s="7"/>
       <c r="S463" s="6"/>
       <c r="T463" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U463" s="6"/>
     </row>
     <row r="464" spans="1:21" outlineLevel="1">
       <c r="A464" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B464" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C464" s="5">
         <v>20</v>
@@ -29792,7 +29795,7 @@
         <v>1</v>
       </c>
       <c r="H464" s="6" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="I464" s="6"/>
       <c r="J464" s="6">
@@ -29816,16 +29819,16 @@
       <c r="R464" s="7"/>
       <c r="S464" s="6"/>
       <c r="T464" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U464" s="6"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29843,7 +29846,7 @@
         <v>2</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29867,16 +29870,16 @@
       <c r="R465" s="7"/>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29894,7 +29897,7 @@
         <v>3</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29918,16 +29921,16 @@
       <c r="R466" s="7"/>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29945,7 +29948,7 @@
         <v>4</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29971,16 +29974,16 @@
       <c r="R467" s="7"/>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29998,7 +30001,7 @@
         <v>0</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30024,18 +30027,18 @@
       <c r="R468" s="7"/>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U468" s="6" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="469" spans="1:21">
       <c r="A469" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C469" s="2">
         <v>60</v>
@@ -30053,7 +30056,7 @@
         <v>0</v>
       </c>
       <c r="H469" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I469" s="2"/>
       <c r="J469" s="2">
@@ -30081,16 +30084,16 @@
         <v>1</v>
       </c>
       <c r="T469" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U469" s="2"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C470" s="5">
         <v>60</v>
@@ -30108,7 +30111,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30132,16 +30135,16 @@
       <c r="R470" s="7"/>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U470" s="6"/>
     </row>
     <row r="471" spans="1:21" outlineLevel="1">
       <c r="A471" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B471" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C471" s="5">
         <v>60</v>
@@ -30159,7 +30162,7 @@
         <v>1</v>
       </c>
       <c r="H471" s="6" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="I471" s="6"/>
       <c r="J471" s="6">
@@ -30183,16 +30186,16 @@
       <c r="R471" s="7"/>
       <c r="S471" s="6"/>
       <c r="T471" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U471" s="6"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30210,7 +30213,7 @@
         <v>2</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30234,16 +30237,16 @@
       <c r="R472" s="7"/>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30261,7 +30264,7 @@
         <v>3</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30285,16 +30288,16 @@
       <c r="R473" s="7"/>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30312,7 +30315,7 @@
         <v>4</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30338,16 +30341,16 @@
       <c r="R474" s="7"/>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30365,7 +30368,7 @@
         <v>0</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30391,18 +30394,18 @@
       <c r="R475" s="7"/>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U475" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="476" spans="1:21">
       <c r="A476" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C476" s="2">
         <v>60</v>
@@ -30420,7 +30423,7 @@
         <v>0</v>
       </c>
       <c r="H476" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="I476" s="2"/>
       <c r="J476" s="2">
@@ -30448,16 +30451,16 @@
         <v>2</v>
       </c>
       <c r="T476" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="U476" s="2"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30475,7 +30478,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30499,16 +30502,16 @@
       <c r="R477" s="7"/>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U477" s="6"/>
     </row>
     <row r="478" spans="1:21" outlineLevel="1">
       <c r="A478" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B478" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C478" s="5">
         <v>60</v>
@@ -30526,7 +30529,7 @@
         <v>1</v>
       </c>
       <c r="H478" s="6" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="I478" s="6"/>
       <c r="J478" s="6">
@@ -30550,16 +30553,16 @@
       <c r="R478" s="7"/>
       <c r="S478" s="6"/>
       <c r="T478" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U478" s="6"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30577,7 +30580,7 @@
         <v>2</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30601,16 +30604,16 @@
       <c r="R479" s="7"/>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30628,7 +30631,7 @@
         <v>3</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30652,16 +30655,16 @@
       <c r="R480" s="7"/>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30679,7 +30682,7 @@
         <v>4</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30705,16 +30708,16 @@
       <c r="R481" s="7"/>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30732,7 +30735,7 @@
         <v>0</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30758,18 +30761,18 @@
       <c r="R482" s="7"/>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U482" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="483" spans="1:21">
       <c r="A483" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C483" s="2">
         <v>60</v>
@@ -30787,7 +30790,7 @@
         <v>0</v>
       </c>
       <c r="H483" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="I483" s="2"/>
       <c r="J483" s="2">
@@ -30815,16 +30818,16 @@
         <v>3</v>
       </c>
       <c r="T483" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="U483" s="2"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30842,7 +30845,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30866,16 +30869,16 @@
       <c r="R484" s="7"/>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U484" s="6"/>
     </row>
     <row r="485" spans="1:21" outlineLevel="1">
       <c r="A485" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B485" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C485" s="5">
         <v>60</v>
@@ -30893,7 +30896,7 @@
         <v>1</v>
       </c>
       <c r="H485" s="6" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="I485" s="6"/>
       <c r="J485" s="6">
@@ -30917,16 +30920,16 @@
       <c r="R485" s="7"/>
       <c r="S485" s="6"/>
       <c r="T485" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U485" s="6"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30944,7 +30947,7 @@
         <v>2</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30968,16 +30971,16 @@
       <c r="R486" s="7"/>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30995,7 +30998,7 @@
         <v>3</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31019,16 +31022,16 @@
       <c r="R487" s="7"/>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31046,7 +31049,7 @@
         <v>4</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31072,16 +31075,16 @@
       <c r="R488" s="7"/>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31099,7 +31102,7 @@
         <v>0</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31125,18 +31128,18 @@
       <c r="R489" s="7"/>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U489" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="490" spans="1:21">
       <c r="A490" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C490" s="2">
         <v>100</v>
@@ -31154,7 +31157,7 @@
         <v>0</v>
       </c>
       <c r="H490" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="I490" s="2"/>
       <c r="J490" s="2">
@@ -31182,16 +31185,16 @@
         <v>4</v>
       </c>
       <c r="T490" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="U490" s="2"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C491" s="5">
         <v>100</v>
@@ -31209,7 +31212,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31233,16 +31236,16 @@
       <c r="R491" s="7"/>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U491" s="6"/>
     </row>
     <row r="492" spans="1:21" outlineLevel="1">
       <c r="A492" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B492" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C492" s="5">
         <v>100</v>
@@ -31260,7 +31263,7 @@
         <v>1</v>
       </c>
       <c r="H492" s="6" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="I492" s="6"/>
       <c r="J492" s="6">
@@ -31284,16 +31287,16 @@
       <c r="R492" s="7"/>
       <c r="S492" s="6"/>
       <c r="T492" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U492" s="6"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31311,7 +31314,7 @@
         <v>2</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31335,16 +31338,16 @@
       <c r="R493" s="7"/>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31362,7 +31365,7 @@
         <v>3</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31386,16 +31389,16 @@
       <c r="R494" s="7"/>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31413,7 +31416,7 @@
         <v>4</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31439,16 +31442,16 @@
       <c r="R495" s="7"/>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31466,7 +31469,7 @@
         <v>0</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31492,18 +31495,18 @@
       <c r="R496" s="7"/>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U496" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="497" spans="1:21">
       <c r="A497" s="2" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C497" s="2">
         <v>60</v>
@@ -31521,7 +31524,7 @@
         <v>0</v>
       </c>
       <c r="H497" s="2" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I497" s="2"/>
       <c r="J497" s="2">
@@ -31549,16 +31552,16 @@
         <v>5</v>
       </c>
       <c r="T497" s="2" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="U497" s="2"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C498" s="5">
         <v>60</v>
@@ -31576,7 +31579,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31600,16 +31603,16 @@
       <c r="R498" s="7"/>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U498" s="6"/>
     </row>
     <row r="499" spans="1:21" outlineLevel="1">
       <c r="A499" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B499" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C499" s="5">
         <v>60</v>
@@ -31627,7 +31630,7 @@
         <v>1</v>
       </c>
       <c r="H499" s="6" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="I499" s="6"/>
       <c r="J499" s="6">
@@ -31651,16 +31654,16 @@
       <c r="R499" s="7"/>
       <c r="S499" s="6"/>
       <c r="T499" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U499" s="6"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31678,7 +31681,7 @@
         <v>2</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31702,16 +31705,16 @@
       <c r="R500" s="7"/>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31729,7 +31732,7 @@
         <v>3</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31753,16 +31756,16 @@
       <c r="R501" s="7"/>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31780,7 +31783,7 @@
         <v>4</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31806,16 +31809,16 @@
       <c r="R502" s="7"/>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31833,7 +31836,7 @@
         <v>0</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31859,18 +31862,18 @@
       <c r="R503" s="7"/>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U503" s="6" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="504" spans="1:21">
       <c r="A504" s="2" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B504" s="2" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C504" s="2">
         <v>100</v>
@@ -31888,7 +31891,7 @@
         <v>0</v>
       </c>
       <c r="H504" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I504" s="2"/>
       <c r="J504" s="2">
@@ -31916,16 +31919,16 @@
         <v>6</v>
       </c>
       <c r="T504" s="2" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="U504" s="2"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C505" s="5">
         <v>100</v>
@@ -31943,7 +31946,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31967,16 +31970,16 @@
       <c r="R505" s="7"/>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U505" s="6"/>
     </row>
     <row r="506" spans="1:21" outlineLevel="1">
       <c r="A506" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B506" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C506" s="5">
         <v>100</v>
@@ -31994,7 +31997,7 @@
         <v>1</v>
       </c>
       <c r="H506" s="6" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="I506" s="6"/>
       <c r="J506" s="6">
@@ -32018,16 +32021,16 @@
       <c r="R506" s="7"/>
       <c r="S506" s="6"/>
       <c r="T506" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U506" s="6"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32045,7 +32048,7 @@
         <v>2</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32069,16 +32072,16 @@
       <c r="R507" s="7"/>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32096,7 +32099,7 @@
         <v>3</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32120,16 +32123,16 @@
       <c r="R508" s="7"/>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32147,7 +32150,7 @@
         <v>4</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32173,16 +32176,16 @@
       <c r="R509" s="7"/>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32200,7 +32203,7 @@
         <v>0</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32226,18 +32229,18 @@
       <c r="R510" s="7"/>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="U510" s="6" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="511" spans="1:21">
       <c r="A511" s="2" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C511" s="2">
         <v>100</v>
@@ -32255,7 +32258,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="2" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I511" s="2"/>
       <c r="J511" s="2">
@@ -32283,16 +32286,16 @@
         <v>7</v>
       </c>
       <c r="T511" s="2" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="U511" s="2"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32310,7 +32313,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32334,16 +32337,16 @@
       <c r="R512" s="7"/>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U512" s="6"/>
     </row>
     <row r="513" spans="1:21" outlineLevel="1">
       <c r="A513" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B513" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C513" s="5">
         <v>100</v>
@@ -32361,7 +32364,7 @@
         <v>1</v>
       </c>
       <c r="H513" s="6" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="I513" s="6"/>
       <c r="J513" s="6">
@@ -32385,16 +32388,16 @@
       <c r="R513" s="7"/>
       <c r="S513" s="6"/>
       <c r="T513" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U513" s="6"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32412,7 +32415,7 @@
         <v>2</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32436,16 +32439,16 @@
       <c r="R514" s="7"/>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32463,7 +32466,7 @@
         <v>3</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32487,16 +32490,16 @@
       <c r="R515" s="7"/>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32514,7 +32517,7 @@
         <v>4</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32540,16 +32543,16 @@
       <c r="R516" s="7"/>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32567,7 +32570,7 @@
         <v>0</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32593,10 +32596,10 @@
       <c r="R517" s="7"/>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="U517" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at c8177f5
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -10,14 +10,14 @@
     <sheet name="K-Matrix " sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$AD$518</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'K-Matrix '!$A$1:$AD$520</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5976" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5998" uniqueCount="1043">
   <si>
     <t>ID</t>
   </si>
@@ -2792,6 +2792,21 @@
   </si>
   <si>
     <t>Lowest measured cell body temperature.</t>
+  </si>
+  <si>
+    <t>HVB_idxCell_tMax</t>
+  </si>
+  <si>
+    <t>Thermistor ID reporting the highest cell body temperature.</t>
+  </si>
+  <si>
+    <t>degC</t>
+  </si>
+  <si>
+    <t>HVB_idxCell_tMin</t>
+  </si>
+  <si>
+    <t>Thermistor ID reporting the lowest cell body temperature.</t>
   </si>
   <si>
     <t>209h</t>
@@ -3519,7 +3534,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U517"/>
+  <dimension ref="A1:U519"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -29066,74 +29081,70 @@
         <v>554</v>
       </c>
     </row>
-    <row r="451" spans="1:21">
-      <c r="A451" s="2" t="s">
+    <row r="451" spans="1:21" outlineLevel="1">
+      <c r="A451" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="B451" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="C451" s="5">
+        <v>100</v>
+      </c>
+      <c r="D451" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E451" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F451" s="6">
+        <v>7</v>
+      </c>
+      <c r="G451" s="6">
+        <v>0</v>
+      </c>
+      <c r="H451" s="6" t="s">
         <v>925</v>
       </c>
-      <c r="B451" s="2" t="s">
+      <c r="I451" s="6" t="s">
         <v>926</v>
       </c>
-      <c r="C451" s="2">
-        <v>200</v>
-      </c>
-      <c r="D451" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="E451" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F451" s="2">
-        <v>2</v>
-      </c>
-      <c r="G451" s="2">
-        <v>0</v>
-      </c>
-      <c r="H451" s="2" t="s">
+      <c r="J451" s="6">
+        <v>8</v>
+      </c>
+      <c r="K451" s="6">
+        <v>0</v>
+      </c>
+      <c r="L451" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M451" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N451" s="7"/>
+      <c r="O451" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P451" s="7"/>
+      <c r="Q451" s="6"/>
+      <c r="R451" s="7"/>
+      <c r="S451" s="6"/>
+      <c r="T451" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U451" s="6" t="s">
         <v>927</v>
       </c>
-      <c r="I451" s="2" t="s">
-        <v>858</v>
-      </c>
-      <c r="J451" s="2">
-        <v>8</v>
-      </c>
-      <c r="K451" s="2">
-        <v>0</v>
-      </c>
-      <c r="L451" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M451" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N451" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O451" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P451" s="3"/>
-      <c r="Q451" s="2"/>
-      <c r="R451" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S451" s="2">
-        <v>0</v>
-      </c>
-      <c r="T451" s="2" t="s">
-        <v>863</v>
-      </c>
-      <c r="U451" s="2"/>
     </row>
     <row r="452" spans="1:21" outlineLevel="1">
       <c r="A452" s="5" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="B452" s="5" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="C452" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D452" s="5" t="s">
         <v>811</v>
@@ -29141,114 +29152,110 @@
       <c r="E452" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F452" s="5">
-        <v>2</v>
-      </c>
-      <c r="G452" s="5">
-        <v>0</v>
-      </c>
-      <c r="H452" s="5" t="s">
-        <v>927</v>
-      </c>
-      <c r="I452" s="5" t="s">
-        <v>858</v>
-      </c>
-      <c r="J452" s="5">
+      <c r="F452" s="6">
         <v>8</v>
       </c>
-      <c r="K452" s="5">
-        <v>0</v>
-      </c>
-      <c r="L452" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M452" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N452" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="G452" s="6">
+        <v>0</v>
+      </c>
+      <c r="H452" s="6" t="s">
+        <v>928</v>
+      </c>
+      <c r="I452" s="6" t="s">
+        <v>929</v>
+      </c>
+      <c r="J452" s="6">
+        <v>8</v>
+      </c>
+      <c r="K452" s="6">
+        <v>0</v>
+      </c>
+      <c r="L452" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M452" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N452" s="7"/>
       <c r="O452" s="8" t="s">
         <v>25</v>
       </c>
       <c r="P452" s="7"/>
       <c r="Q452" s="6"/>
-      <c r="R452" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="S452" s="6">
-        <v>1</v>
-      </c>
+      <c r="R452" s="7"/>
+      <c r="S452" s="6"/>
       <c r="T452" s="6" t="s">
-        <v>928</v>
-      </c>
-      <c r="U452" s="5"/>
-    </row>
-    <row r="453" spans="1:21" outlineLevel="1">
-      <c r="A453" s="5" t="s">
-        <v>925</v>
-      </c>
-      <c r="B453" s="5" t="s">
-        <v>926</v>
-      </c>
-      <c r="C453" s="5">
+        <v>31</v>
+      </c>
+      <c r="U452" s="6" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="453" spans="1:21">
+      <c r="A453" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B453" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="C453" s="2">
         <v>200</v>
       </c>
-      <c r="D453" s="5" t="s">
+      <c r="D453" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E453" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F453" s="5">
+      <c r="E453" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F453" s="2">
         <v>2</v>
       </c>
-      <c r="G453" s="5">
-        <v>0</v>
-      </c>
-      <c r="H453" s="5" t="s">
-        <v>927</v>
-      </c>
-      <c r="I453" s="5" t="s">
+      <c r="G453" s="2">
+        <v>0</v>
+      </c>
+      <c r="H453" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="I453" s="2" t="s">
         <v>858</v>
       </c>
-      <c r="J453" s="5">
+      <c r="J453" s="2">
         <v>8</v>
       </c>
-      <c r="K453" s="5">
-        <v>0</v>
-      </c>
-      <c r="L453" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M453" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N453" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="O453" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P453" s="7"/>
-      <c r="Q453" s="6"/>
-      <c r="R453" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="S453" s="6">
-        <v>2</v>
-      </c>
-      <c r="T453" s="6" t="s">
-        <v>929</v>
-      </c>
-      <c r="U453" s="5"/>
+      <c r="K453" s="2">
+        <v>0</v>
+      </c>
+      <c r="L453" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M453" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N453" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O453" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P453" s="3"/>
+      <c r="Q453" s="2"/>
+      <c r="R453" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S453" s="2">
+        <v>0</v>
+      </c>
+      <c r="T453" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="U453" s="2"/>
     </row>
     <row r="454" spans="1:21" outlineLevel="1">
       <c r="A454" s="5" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="B454" s="5" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="C454" s="5">
         <v>200</v>
@@ -29266,7 +29273,7 @@
         <v>0</v>
       </c>
       <c r="H454" s="5" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="I454" s="5" t="s">
         <v>858</v>
@@ -29295,19 +29302,19 @@
         <v>26</v>
       </c>
       <c r="S454" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="U454" s="5"/>
     </row>
     <row r="455" spans="1:21" outlineLevel="1">
       <c r="A455" s="5" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="B455" s="5" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="C455" s="5">
         <v>200</v>
@@ -29325,7 +29332,7 @@
         <v>0</v>
       </c>
       <c r="H455" s="5" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="I455" s="5" t="s">
         <v>858</v>
@@ -29354,19 +29361,19 @@
         <v>26</v>
       </c>
       <c r="S455" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="U455" s="5"/>
     </row>
     <row r="456" spans="1:21" outlineLevel="1">
       <c r="A456" s="5" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="B456" s="5" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="C456" s="5">
         <v>200</v>
@@ -29384,7 +29391,7 @@
         <v>0</v>
       </c>
       <c r="H456" s="5" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="I456" s="5" t="s">
         <v>858</v>
@@ -29413,19 +29420,19 @@
         <v>26</v>
       </c>
       <c r="S456" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="U456" s="5"/>
     </row>
     <row r="457" spans="1:21" outlineLevel="1">
       <c r="A457" s="5" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="B457" s="5" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="C457" s="5">
         <v>200</v>
@@ -29436,28 +29443,28 @@
       <c r="E457" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F457" s="6">
-        <v>5</v>
-      </c>
-      <c r="G457" s="6">
-        <v>0</v>
-      </c>
-      <c r="H457" s="6" t="s">
-        <v>933</v>
-      </c>
-      <c r="I457" s="6" t="s">
-        <v>934</v>
-      </c>
-      <c r="J457" s="6">
-        <v>16</v>
-      </c>
-      <c r="K457" s="6">
-        <v>0</v>
-      </c>
-      <c r="L457" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M457" s="6" t="s">
+      <c r="F457" s="5">
+        <v>2</v>
+      </c>
+      <c r="G457" s="5">
+        <v>0</v>
+      </c>
+      <c r="H457" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="I457" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="J457" s="5">
+        <v>8</v>
+      </c>
+      <c r="K457" s="5">
+        <v>0</v>
+      </c>
+      <c r="L457" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M457" s="5" t="s">
         <v>30</v>
       </c>
       <c r="N457" s="7" t="s">
@@ -29471,80 +29478,82 @@
       <c r="R457" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="S457" s="6"/>
+      <c r="S457" s="6">
+        <v>4</v>
+      </c>
       <c r="T457" s="6" t="s">
-        <v>935</v>
-      </c>
-      <c r="U457" s="6" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="458" spans="1:21">
-      <c r="A458" s="2" t="s">
+      <c r="U457" s="5"/>
+    </row>
+    <row r="458" spans="1:21" outlineLevel="1">
+      <c r="A458" s="5" t="s">
+        <v>930</v>
+      </c>
+      <c r="B458" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="C458" s="5">
+        <v>200</v>
+      </c>
+      <c r="D458" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E458" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F458" s="5">
+        <v>2</v>
+      </c>
+      <c r="G458" s="5">
+        <v>0</v>
+      </c>
+      <c r="H458" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="I458" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="J458" s="5">
+        <v>8</v>
+      </c>
+      <c r="K458" s="5">
+        <v>0</v>
+      </c>
+      <c r="L458" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M458" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N458" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O458" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P458" s="7"/>
+      <c r="Q458" s="6"/>
+      <c r="R458" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S458" s="6">
+        <v>6</v>
+      </c>
+      <c r="T458" s="6" t="s">
         <v>937</v>
       </c>
-      <c r="B458" s="2" t="s">
-        <v>938</v>
-      </c>
-      <c r="C458" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D458" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="E458" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F458" s="2">
-        <v>1</v>
-      </c>
-      <c r="G458" s="2">
-        <v>0</v>
-      </c>
-      <c r="H458" s="2" t="s">
-        <v>939</v>
-      </c>
-      <c r="I458" s="2" t="s">
-        <v>940</v>
-      </c>
-      <c r="J458" s="2">
-        <v>32</v>
-      </c>
-      <c r="K458" s="2">
-        <v>0</v>
-      </c>
-      <c r="L458" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M458" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N458" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O458" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P458" s="3"/>
-      <c r="Q458" s="2"/>
-      <c r="R458" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S458" s="2"/>
-      <c r="T458" s="2" t="s">
-        <v>941</v>
-      </c>
-      <c r="U458" s="2"/>
+      <c r="U458" s="5"/>
     </row>
     <row r="459" spans="1:21" outlineLevel="1">
       <c r="A459" s="5" t="s">
-        <v>937</v>
+        <v>930</v>
       </c>
       <c r="B459" s="5" t="s">
-        <v>938</v>
+        <v>931</v>
       </c>
       <c r="C459" s="5">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="D459" s="5" t="s">
         <v>811</v>
@@ -29559,13 +29568,13 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="J459" s="6">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="K459" s="6">
         <v>0</v>
@@ -29589,243 +29598,257 @@
       </c>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="U459" s="6" t="s">
         <v>941</v>
       </c>
-      <c r="U459" s="6"/>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>943</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="C460" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D460" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="E460" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F460" s="2">
+        <v>1</v>
+      </c>
+      <c r="G460" s="2">
+        <v>0</v>
+      </c>
+      <c r="H460" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="C460" s="2">
-        <v>0</v>
-      </c>
-      <c r="D460" s="2" t="s">
+      <c r="I460" s="2" t="s">
         <v>945</v>
       </c>
-      <c r="E460" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F460" s="2"/>
-      <c r="G460" s="2"/>
-      <c r="H460" s="2"/>
-      <c r="I460" s="2"/>
-      <c r="J460" s="2"/>
-      <c r="K460" s="2"/>
-      <c r="L460" s="2"/>
-      <c r="M460" s="2"/>
-      <c r="N460" s="3"/>
+      <c r="J460" s="2">
+        <v>32</v>
+      </c>
+      <c r="K460" s="2">
+        <v>0</v>
+      </c>
+      <c r="L460" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M460" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N460" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="O460" s="4" t="s">
         <v>25</v>
       </c>
       <c r="P460" s="3"/>
       <c r="Q460" s="2"/>
-      <c r="R460" s="3"/>
+      <c r="R460" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="S460" s="2"/>
-      <c r="T460" s="2"/>
+      <c r="T460" s="2" t="s">
+        <v>946</v>
+      </c>
       <c r="U460" s="2"/>
     </row>
-    <row r="461" spans="1:21">
-      <c r="A461" s="2" t="s">
+    <row r="461" spans="1:21" outlineLevel="1">
+      <c r="A461" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="B461" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="C461" s="5">
+        <v>1000</v>
+      </c>
+      <c r="D461" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E461" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F461" s="6">
+        <v>5</v>
+      </c>
+      <c r="G461" s="6">
+        <v>0</v>
+      </c>
+      <c r="H461" s="6" t="s">
+        <v>947</v>
+      </c>
+      <c r="I461" s="6" t="s">
+        <v>945</v>
+      </c>
+      <c r="J461" s="6">
+        <v>32</v>
+      </c>
+      <c r="K461" s="6">
+        <v>0</v>
+      </c>
+      <c r="L461" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M461" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N461" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O461" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P461" s="7"/>
+      <c r="Q461" s="6"/>
+      <c r="R461" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S461" s="6"/>
+      <c r="T461" s="6" t="s">
         <v>946</v>
       </c>
-      <c r="B461" s="2" t="s">
-        <v>947</v>
-      </c>
-      <c r="C461" s="2">
-        <v>0</v>
-      </c>
-      <c r="D461" s="2" t="s">
-        <v>948</v>
-      </c>
-      <c r="E461" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F461" s="2"/>
-      <c r="G461" s="2"/>
-      <c r="H461" s="2"/>
-      <c r="I461" s="2"/>
-      <c r="J461" s="2"/>
-      <c r="K461" s="2"/>
-      <c r="L461" s="2"/>
-      <c r="M461" s="2"/>
-      <c r="N461" s="3"/>
-      <c r="O461" s="2"/>
-      <c r="P461" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q461" s="2"/>
-      <c r="R461" s="3"/>
-      <c r="S461" s="2"/>
-      <c r="T461" s="2"/>
-      <c r="U461" s="2"/>
+      <c r="U461" s="6"/>
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>949</v>
       </c>
-      <c r="B462" s="2" t="s">
+      <c r="C462" s="2">
+        <v>0</v>
+      </c>
+      <c r="D462" s="2" t="s">
         <v>950</v>
       </c>
-      <c r="C462" s="2">
-        <v>20</v>
-      </c>
-      <c r="D462" s="2" t="s">
-        <v>811</v>
-      </c>
       <c r="E462" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F462" s="2">
-        <v>1</v>
-      </c>
-      <c r="G462" s="2">
-        <v>0</v>
-      </c>
-      <c r="H462" s="2" t="s">
-        <v>951</v>
-      </c>
+      <c r="F462" s="2"/>
+      <c r="G462" s="2"/>
+      <c r="H462" s="2"/>
       <c r="I462" s="2"/>
-      <c r="J462" s="2">
-        <v>8</v>
-      </c>
-      <c r="K462" s="2">
-        <v>0</v>
-      </c>
-      <c r="L462" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M462" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="J462" s="2"/>
+      <c r="K462" s="2"/>
+      <c r="L462" s="2"/>
+      <c r="M462" s="2"/>
       <c r="N462" s="3"/>
-      <c r="O462" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P462" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="O462" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P462" s="3"/>
       <c r="Q462" s="2"/>
       <c r="R462" s="3"/>
-      <c r="S462" s="2">
-        <v>0</v>
-      </c>
-      <c r="T462" s="2" t="s">
+      <c r="S462" s="2"/>
+      <c r="T462" s="2"/>
+      <c r="U462" s="2"/>
+    </row>
+    <row r="463" spans="1:21">
+      <c r="A463" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="B463" s="2" t="s">
         <v>952</v>
       </c>
-      <c r="U462" s="2"/>
-    </row>
-    <row r="463" spans="1:21" outlineLevel="1">
-      <c r="A463" s="5" t="s">
-        <v>949</v>
-      </c>
-      <c r="B463" s="5" t="s">
-        <v>950</v>
-      </c>
-      <c r="C463" s="5">
+      <c r="C463" s="2">
+        <v>0</v>
+      </c>
+      <c r="D463" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="E463" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F463" s="2"/>
+      <c r="G463" s="2"/>
+      <c r="H463" s="2"/>
+      <c r="I463" s="2"/>
+      <c r="J463" s="2"/>
+      <c r="K463" s="2"/>
+      <c r="L463" s="2"/>
+      <c r="M463" s="2"/>
+      <c r="N463" s="3"/>
+      <c r="O463" s="2"/>
+      <c r="P463" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q463" s="2"/>
+      <c r="R463" s="3"/>
+      <c r="S463" s="2"/>
+      <c r="T463" s="2"/>
+      <c r="U463" s="2"/>
+    </row>
+    <row r="464" spans="1:21">
+      <c r="A464" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B464" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="C464" s="2">
         <v>20</v>
       </c>
-      <c r="D463" s="5" t="s">
+      <c r="D464" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E463" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F463" s="6">
-        <v>2</v>
-      </c>
-      <c r="G463" s="6">
-        <v>0</v>
-      </c>
-      <c r="H463" s="6" t="s">
-        <v>953</v>
-      </c>
-      <c r="I463" s="6"/>
-      <c r="J463" s="6">
+      <c r="E464" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F464" s="2">
         <v>1</v>
       </c>
-      <c r="K463" s="6">
-        <v>0</v>
-      </c>
-      <c r="L463" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M463" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N463" s="7"/>
-      <c r="O463" s="6"/>
-      <c r="P463" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q463" s="6"/>
-      <c r="R463" s="7"/>
-      <c r="S463" s="6"/>
-      <c r="T463" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U463" s="6"/>
-    </row>
-    <row r="464" spans="1:21" outlineLevel="1">
-      <c r="A464" s="5" t="s">
-        <v>949</v>
-      </c>
-      <c r="B464" s="5" t="s">
-        <v>950</v>
-      </c>
-      <c r="C464" s="5">
-        <v>20</v>
-      </c>
-      <c r="D464" s="5" t="s">
-        <v>811</v>
-      </c>
-      <c r="E464" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F464" s="6">
-        <v>2</v>
-      </c>
-      <c r="G464" s="6">
-        <v>1</v>
-      </c>
-      <c r="H464" s="6" t="s">
-        <v>955</v>
-      </c>
-      <c r="I464" s="6"/>
-      <c r="J464" s="6">
-        <v>1</v>
-      </c>
-      <c r="K464" s="6">
-        <v>0</v>
-      </c>
-      <c r="L464" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M464" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N464" s="7"/>
-      <c r="O464" s="6"/>
-      <c r="P464" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q464" s="6"/>
-      <c r="R464" s="7"/>
-      <c r="S464" s="6"/>
-      <c r="T464" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U464" s="6"/>
+      <c r="G464" s="2">
+        <v>0</v>
+      </c>
+      <c r="H464" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="I464" s="2"/>
+      <c r="J464" s="2">
+        <v>8</v>
+      </c>
+      <c r="K464" s="2">
+        <v>0</v>
+      </c>
+      <c r="L464" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M464" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N464" s="3"/>
+      <c r="O464" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P464" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q464" s="2"/>
+      <c r="R464" s="3"/>
+      <c r="S464" s="2">
+        <v>0</v>
+      </c>
+      <c r="T464" s="2" t="s">
+        <v>957</v>
+      </c>
+      <c r="U464" s="2"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29840,10 +29863,10 @@
         <v>2</v>
       </c>
       <c r="G465" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29867,16 +29890,16 @@
       <c r="R465" s="7"/>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29891,10 +29914,10 @@
         <v>2</v>
       </c>
       <c r="G466" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29918,16 +29941,16 @@
       <c r="R466" s="7"/>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29942,14 +29965,14 @@
         <v>2</v>
       </c>
       <c r="G467" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>958</v>
+        <v>961</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K467" s="6">
         <v>0</v>
@@ -29961,9 +29984,7 @@
         <v>30</v>
       </c>
       <c r="N467" s="7"/>
-      <c r="O467" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O467" s="6"/>
       <c r="P467" s="10" t="s">
         <v>25</v>
       </c>
@@ -29971,16 +29992,16 @@
       <c r="R467" s="7"/>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -29992,17 +30013,17 @@
         <v>24</v>
       </c>
       <c r="F468" s="6">
+        <v>2</v>
+      </c>
+      <c r="G468" s="6">
         <v>3</v>
       </c>
-      <c r="G468" s="6">
-        <v>0</v>
-      </c>
       <c r="H468" s="6" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K468" s="6">
         <v>0</v>
@@ -30014,9 +30035,7 @@
         <v>30</v>
       </c>
       <c r="N468" s="7"/>
-      <c r="O468" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O468" s="6"/>
       <c r="P468" s="10" t="s">
         <v>25</v>
       </c>
@@ -30024,76 +30043,72 @@
       <c r="R468" s="7"/>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="U468" s="6" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="469" spans="1:21">
-      <c r="A469" s="2" t="s">
-        <v>962</v>
-      </c>
-      <c r="B469" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="U468" s="6"/>
+    </row>
+    <row r="469" spans="1:21" outlineLevel="1">
+      <c r="A469" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B469" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C469" s="5">
+        <v>20</v>
+      </c>
+      <c r="D469" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E469" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F469" s="6">
+        <v>2</v>
+      </c>
+      <c r="G469" s="6">
+        <v>4</v>
+      </c>
+      <c r="H469" s="6" t="s">
         <v>963</v>
       </c>
-      <c r="C469" s="2">
-        <v>60</v>
-      </c>
-      <c r="D469" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="E469" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F469" s="2">
-        <v>1</v>
-      </c>
-      <c r="G469" s="2">
-        <v>0</v>
-      </c>
-      <c r="H469" s="2" t="s">
-        <v>964</v>
-      </c>
-      <c r="I469" s="2"/>
-      <c r="J469" s="2">
-        <v>8</v>
-      </c>
-      <c r="K469" s="2">
-        <v>1</v>
-      </c>
-      <c r="L469" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M469" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N469" s="3"/>
-      <c r="O469" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P469" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q469" s="2"/>
-      <c r="R469" s="3"/>
-      <c r="S469" s="2">
-        <v>1</v>
-      </c>
-      <c r="T469" s="2" t="s">
-        <v>965</v>
-      </c>
-      <c r="U469" s="2"/>
+      <c r="I469" s="6"/>
+      <c r="J469" s="6">
+        <v>4</v>
+      </c>
+      <c r="K469" s="6">
+        <v>0</v>
+      </c>
+      <c r="L469" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M469" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N469" s="7"/>
+      <c r="O469" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P469" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q469" s="6"/>
+      <c r="R469" s="7"/>
+      <c r="S469" s="6"/>
+      <c r="T469" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U469" s="6"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
       <c r="C470" s="5">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D470" s="5" t="s">
         <v>811</v>
@@ -30102,17 +30117,17 @@
         <v>24</v>
       </c>
       <c r="F470" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G470" s="6">
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K470" s="6">
         <v>0</v>
@@ -30124,7 +30139,9 @@
         <v>30</v>
       </c>
       <c r="N470" s="7"/>
-      <c r="O470" s="6"/>
+      <c r="O470" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="P470" s="10" t="s">
         <v>25</v>
       </c>
@@ -30132,67 +30149,73 @@
       <c r="R470" s="7"/>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U470" s="6"/>
-    </row>
-    <row r="471" spans="1:21" outlineLevel="1">
-      <c r="A471" s="5" t="s">
-        <v>962</v>
-      </c>
-      <c r="B471" s="5" t="s">
-        <v>963</v>
-      </c>
-      <c r="C471" s="5">
+        <v>965</v>
+      </c>
+      <c r="U470" s="6" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="471" spans="1:21">
+      <c r="A471" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="C471" s="2">
         <v>60</v>
       </c>
-      <c r="D471" s="5" t="s">
+      <c r="D471" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E471" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F471" s="6">
-        <v>2</v>
-      </c>
-      <c r="G471" s="6">
+      <c r="E471" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F471" s="2">
         <v>1</v>
       </c>
-      <c r="H471" s="6" t="s">
-        <v>967</v>
-      </c>
-      <c r="I471" s="6"/>
-      <c r="J471" s="6">
+      <c r="G471" s="2">
+        <v>0</v>
+      </c>
+      <c r="H471" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="I471" s="2"/>
+      <c r="J471" s="2">
+        <v>8</v>
+      </c>
+      <c r="K471" s="2">
         <v>1</v>
       </c>
-      <c r="K471" s="6">
-        <v>0</v>
-      </c>
-      <c r="L471" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M471" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N471" s="7"/>
-      <c r="O471" s="6"/>
-      <c r="P471" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q471" s="6"/>
-      <c r="R471" s="7"/>
-      <c r="S471" s="6"/>
-      <c r="T471" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U471" s="6"/>
+      <c r="L471" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M471" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N471" s="3"/>
+      <c r="O471" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P471" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q471" s="2"/>
+      <c r="R471" s="3"/>
+      <c r="S471" s="2">
+        <v>1</v>
+      </c>
+      <c r="T471" s="2" t="s">
+        <v>970</v>
+      </c>
+      <c r="U471" s="2"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>962</v>
+        <v>967</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30207,10 +30230,10 @@
         <v>2</v>
       </c>
       <c r="G472" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30234,16 +30257,16 @@
       <c r="R472" s="7"/>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>962</v>
+        <v>967</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30258,10 +30281,10 @@
         <v>2</v>
       </c>
       <c r="G473" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30285,16 +30308,16 @@
       <c r="R473" s="7"/>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>962</v>
+        <v>967</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30309,14 +30332,14 @@
         <v>2</v>
       </c>
       <c r="G474" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K474" s="6">
         <v>0</v>
@@ -30328,9 +30351,7 @@
         <v>30</v>
       </c>
       <c r="N474" s="7"/>
-      <c r="O474" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O474" s="6"/>
       <c r="P474" s="10" t="s">
         <v>25</v>
       </c>
@@ -30338,16 +30359,16 @@
       <c r="R474" s="7"/>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>962</v>
+        <v>967</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30359,17 +30380,17 @@
         <v>24</v>
       </c>
       <c r="F475" s="6">
+        <v>2</v>
+      </c>
+      <c r="G475" s="6">
         <v>3</v>
       </c>
-      <c r="G475" s="6">
-        <v>0</v>
-      </c>
       <c r="H475" s="6" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K475" s="6">
         <v>0</v>
@@ -30381,9 +30402,7 @@
         <v>30</v>
       </c>
       <c r="N475" s="7"/>
-      <c r="O475" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O475" s="6"/>
       <c r="P475" s="10" t="s">
         <v>25</v>
       </c>
@@ -30391,73 +30410,69 @@
       <c r="R475" s="7"/>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="U475" s="6" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="476" spans="1:21">
-      <c r="A476" s="2" t="s">
-        <v>973</v>
-      </c>
-      <c r="B476" s="2" t="s">
-        <v>974</v>
-      </c>
-      <c r="C476" s="2">
+        <v>959</v>
+      </c>
+      <c r="U475" s="6"/>
+    </row>
+    <row r="476" spans="1:21" outlineLevel="1">
+      <c r="A476" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B476" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="C476" s="5">
         <v>60</v>
       </c>
-      <c r="D476" s="2" t="s">
+      <c r="D476" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="E476" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F476" s="2">
-        <v>1</v>
-      </c>
-      <c r="G476" s="2">
-        <v>0</v>
-      </c>
-      <c r="H476" s="2" t="s">
+      <c r="E476" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F476" s="6">
+        <v>2</v>
+      </c>
+      <c r="G476" s="6">
+        <v>4</v>
+      </c>
+      <c r="H476" s="6" t="s">
         <v>975</v>
       </c>
-      <c r="I476" s="2"/>
-      <c r="J476" s="2">
-        <v>8</v>
-      </c>
-      <c r="K476" s="2">
-        <v>2</v>
-      </c>
-      <c r="L476" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M476" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N476" s="3"/>
-      <c r="O476" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P476" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q476" s="2"/>
-      <c r="R476" s="3"/>
-      <c r="S476" s="2">
-        <v>2</v>
-      </c>
-      <c r="T476" s="2" t="s">
-        <v>976</v>
-      </c>
-      <c r="U476" s="2"/>
+      <c r="I476" s="6"/>
+      <c r="J476" s="6">
+        <v>4</v>
+      </c>
+      <c r="K476" s="6">
+        <v>0</v>
+      </c>
+      <c r="L476" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M476" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N476" s="7"/>
+      <c r="O476" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P476" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q476" s="6"/>
+      <c r="R476" s="7"/>
+      <c r="S476" s="6"/>
+      <c r="T476" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U476" s="6"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30469,17 +30484,17 @@
         <v>24</v>
       </c>
       <c r="F477" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G477" s="6">
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K477" s="6">
         <v>0</v>
@@ -30491,7 +30506,9 @@
         <v>30</v>
       </c>
       <c r="N477" s="7"/>
-      <c r="O477" s="6"/>
+      <c r="O477" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="P477" s="10" t="s">
         <v>25</v>
       </c>
@@ -30499,67 +30516,73 @@
       <c r="R477" s="7"/>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U477" s="6"/>
-    </row>
-    <row r="478" spans="1:21" outlineLevel="1">
-      <c r="A478" s="5" t="s">
-        <v>973</v>
-      </c>
-      <c r="B478" s="5" t="s">
-        <v>974</v>
-      </c>
-      <c r="C478" s="5">
+        <v>965</v>
+      </c>
+      <c r="U477" s="6" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="478" spans="1:21">
+      <c r="A478" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B478" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="C478" s="2">
         <v>60</v>
       </c>
-      <c r="D478" s="5" t="s">
+      <c r="D478" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E478" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F478" s="6">
+      <c r="E478" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F478" s="2">
+        <v>1</v>
+      </c>
+      <c r="G478" s="2">
+        <v>0</v>
+      </c>
+      <c r="H478" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="I478" s="2"/>
+      <c r="J478" s="2">
+        <v>8</v>
+      </c>
+      <c r="K478" s="2">
         <v>2</v>
       </c>
-      <c r="G478" s="6">
-        <v>1</v>
-      </c>
-      <c r="H478" s="6" t="s">
-        <v>978</v>
-      </c>
-      <c r="I478" s="6"/>
-      <c r="J478" s="6">
-        <v>1</v>
-      </c>
-      <c r="K478" s="6">
-        <v>0</v>
-      </c>
-      <c r="L478" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M478" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N478" s="7"/>
-      <c r="O478" s="6"/>
-      <c r="P478" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q478" s="6"/>
-      <c r="R478" s="7"/>
-      <c r="S478" s="6"/>
-      <c r="T478" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U478" s="6"/>
+      <c r="L478" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M478" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N478" s="3"/>
+      <c r="O478" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P478" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q478" s="2"/>
+      <c r="R478" s="3"/>
+      <c r="S478" s="2">
+        <v>2</v>
+      </c>
+      <c r="T478" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="U478" s="2"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>973</v>
+        <v>978</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>974</v>
+        <v>979</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30574,10 +30597,10 @@
         <v>2</v>
       </c>
       <c r="G479" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30601,16 +30624,16 @@
       <c r="R479" s="7"/>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>973</v>
+        <v>978</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>974</v>
+        <v>979</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30625,10 +30648,10 @@
         <v>2</v>
       </c>
       <c r="G480" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30652,16 +30675,16 @@
       <c r="R480" s="7"/>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>973</v>
+        <v>978</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>974</v>
+        <v>979</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30676,14 +30699,14 @@
         <v>2</v>
       </c>
       <c r="G481" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K481" s="6">
         <v>0</v>
@@ -30695,9 +30718,7 @@
         <v>30</v>
       </c>
       <c r="N481" s="7"/>
-      <c r="O481" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O481" s="6"/>
       <c r="P481" s="10" t="s">
         <v>25</v>
       </c>
@@ -30705,16 +30726,16 @@
       <c r="R481" s="7"/>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>973</v>
+        <v>978</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>974</v>
+        <v>979</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30726,17 +30747,17 @@
         <v>24</v>
       </c>
       <c r="F482" s="6">
+        <v>2</v>
+      </c>
+      <c r="G482" s="6">
         <v>3</v>
       </c>
-      <c r="G482" s="6">
-        <v>0</v>
-      </c>
       <c r="H482" s="6" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K482" s="6">
         <v>0</v>
@@ -30748,9 +30769,7 @@
         <v>30</v>
       </c>
       <c r="N482" s="7"/>
-      <c r="O482" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O482" s="6"/>
       <c r="P482" s="10" t="s">
         <v>25</v>
       </c>
@@ -30758,73 +30777,69 @@
       <c r="R482" s="7"/>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="U482" s="6" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="483" spans="1:21">
-      <c r="A483" s="2" t="s">
-        <v>983</v>
-      </c>
-      <c r="B483" s="2" t="s">
-        <v>984</v>
-      </c>
-      <c r="C483" s="2">
+        <v>959</v>
+      </c>
+      <c r="U482" s="6"/>
+    </row>
+    <row r="483" spans="1:21" outlineLevel="1">
+      <c r="A483" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B483" s="5" t="s">
+        <v>979</v>
+      </c>
+      <c r="C483" s="5">
         <v>60</v>
       </c>
-      <c r="D483" s="2" t="s">
+      <c r="D483" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="E483" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F483" s="2">
-        <v>1</v>
-      </c>
-      <c r="G483" s="2">
-        <v>0</v>
-      </c>
-      <c r="H483" s="2" t="s">
-        <v>985</v>
-      </c>
-      <c r="I483" s="2"/>
-      <c r="J483" s="2">
-        <v>8</v>
-      </c>
-      <c r="K483" s="2">
-        <v>3</v>
-      </c>
-      <c r="L483" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M483" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N483" s="3"/>
-      <c r="O483" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P483" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q483" s="2"/>
-      <c r="R483" s="3"/>
-      <c r="S483" s="2">
-        <v>3</v>
-      </c>
-      <c r="T483" s="2" t="s">
+      <c r="E483" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F483" s="6">
+        <v>2</v>
+      </c>
+      <c r="G483" s="6">
+        <v>4</v>
+      </c>
+      <c r="H483" s="6" t="s">
         <v>986</v>
       </c>
-      <c r="U483" s="2"/>
+      <c r="I483" s="6"/>
+      <c r="J483" s="6">
+        <v>4</v>
+      </c>
+      <c r="K483" s="6">
+        <v>0</v>
+      </c>
+      <c r="L483" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M483" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N483" s="7"/>
+      <c r="O483" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P483" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q483" s="6"/>
+      <c r="R483" s="7"/>
+      <c r="S483" s="6"/>
+      <c r="T483" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U483" s="6"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>983</v>
+        <v>978</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>984</v>
+        <v>979</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30836,7 +30851,7 @@
         <v>24</v>
       </c>
       <c r="F484" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G484" s="6">
         <v>0</v>
@@ -30846,7 +30861,7 @@
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K484" s="6">
         <v>0</v>
@@ -30858,7 +30873,9 @@
         <v>30</v>
       </c>
       <c r="N484" s="7"/>
-      <c r="O484" s="6"/>
+      <c r="O484" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="P484" s="10" t="s">
         <v>25</v>
       </c>
@@ -30866,67 +30883,73 @@
       <c r="R484" s="7"/>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U484" s="6"/>
-    </row>
-    <row r="485" spans="1:21" outlineLevel="1">
-      <c r="A485" s="5" t="s">
-        <v>983</v>
-      </c>
-      <c r="B485" s="5" t="s">
-        <v>984</v>
-      </c>
-      <c r="C485" s="5">
+        <v>965</v>
+      </c>
+      <c r="U484" s="6" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="485" spans="1:21">
+      <c r="A485" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B485" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="C485" s="2">
         <v>60</v>
       </c>
-      <c r="D485" s="5" t="s">
+      <c r="D485" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E485" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F485" s="6">
-        <v>2</v>
-      </c>
-      <c r="G485" s="6">
+      <c r="E485" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F485" s="2">
         <v>1</v>
       </c>
-      <c r="H485" s="6" t="s">
-        <v>988</v>
-      </c>
-      <c r="I485" s="6"/>
-      <c r="J485" s="6">
-        <v>1</v>
-      </c>
-      <c r="K485" s="6">
-        <v>0</v>
-      </c>
-      <c r="L485" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M485" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N485" s="7"/>
-      <c r="O485" s="6"/>
-      <c r="P485" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q485" s="6"/>
-      <c r="R485" s="7"/>
-      <c r="S485" s="6"/>
-      <c r="T485" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U485" s="6"/>
+      <c r="G485" s="2">
+        <v>0</v>
+      </c>
+      <c r="H485" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="I485" s="2"/>
+      <c r="J485" s="2">
+        <v>8</v>
+      </c>
+      <c r="K485" s="2">
+        <v>3</v>
+      </c>
+      <c r="L485" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M485" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N485" s="3"/>
+      <c r="O485" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P485" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q485" s="2"/>
+      <c r="R485" s="3"/>
+      <c r="S485" s="2">
+        <v>3</v>
+      </c>
+      <c r="T485" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="U485" s="2"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>983</v>
+        <v>988</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>984</v>
+        <v>989</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30941,10 +30964,10 @@
         <v>2</v>
       </c>
       <c r="G486" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>989</v>
+        <v>992</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30968,16 +30991,16 @@
       <c r="R486" s="7"/>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>983</v>
+        <v>988</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>984</v>
+        <v>989</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -30992,10 +31015,10 @@
         <v>2</v>
       </c>
       <c r="G487" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31019,16 +31042,16 @@
       <c r="R487" s="7"/>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>983</v>
+        <v>988</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>984</v>
+        <v>989</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31043,14 +31066,14 @@
         <v>2</v>
       </c>
       <c r="G488" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K488" s="6">
         <v>0</v>
@@ -31062,9 +31085,7 @@
         <v>30</v>
       </c>
       <c r="N488" s="7"/>
-      <c r="O488" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O488" s="6"/>
       <c r="P488" s="10" t="s">
         <v>25</v>
       </c>
@@ -31072,16 +31093,16 @@
       <c r="R488" s="7"/>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>983</v>
+        <v>988</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>984</v>
+        <v>989</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31093,17 +31114,17 @@
         <v>24</v>
       </c>
       <c r="F489" s="6">
+        <v>2</v>
+      </c>
+      <c r="G489" s="6">
         <v>3</v>
       </c>
-      <c r="G489" s="6">
-        <v>0</v>
-      </c>
       <c r="H489" s="6" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K489" s="6">
         <v>0</v>
@@ -31115,9 +31136,7 @@
         <v>30</v>
       </c>
       <c r="N489" s="7"/>
-      <c r="O489" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O489" s="6"/>
       <c r="P489" s="10" t="s">
         <v>25</v>
       </c>
@@ -31125,76 +31144,72 @@
       <c r="R489" s="7"/>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="U489" s="6" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="490" spans="1:21">
-      <c r="A490" s="2" t="s">
-        <v>993</v>
-      </c>
-      <c r="B490" s="2" t="s">
-        <v>994</v>
-      </c>
-      <c r="C490" s="2">
-        <v>100</v>
-      </c>
-      <c r="D490" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="U489" s="6"/>
+    </row>
+    <row r="490" spans="1:21" outlineLevel="1">
+      <c r="A490" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B490" s="5" t="s">
+        <v>989</v>
+      </c>
+      <c r="C490" s="5">
+        <v>60</v>
+      </c>
+      <c r="D490" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="E490" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F490" s="2">
-        <v>1</v>
-      </c>
-      <c r="G490" s="2">
-        <v>0</v>
-      </c>
-      <c r="H490" s="2" t="s">
-        <v>995</v>
-      </c>
-      <c r="I490" s="2"/>
-      <c r="J490" s="2">
-        <v>8</v>
-      </c>
-      <c r="K490" s="2">
+      <c r="E490" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F490" s="6">
+        <v>2</v>
+      </c>
+      <c r="G490" s="6">
         <v>4</v>
       </c>
-      <c r="L490" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M490" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N490" s="3"/>
-      <c r="O490" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P490" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q490" s="2"/>
-      <c r="R490" s="3"/>
-      <c r="S490" s="2">
+      <c r="H490" s="6" t="s">
+        <v>996</v>
+      </c>
+      <c r="I490" s="6"/>
+      <c r="J490" s="6">
         <v>4</v>
       </c>
-      <c r="T490" s="2" t="s">
-        <v>996</v>
-      </c>
-      <c r="U490" s="2"/>
+      <c r="K490" s="6">
+        <v>0</v>
+      </c>
+      <c r="L490" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M490" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N490" s="7"/>
+      <c r="O490" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P490" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q490" s="6"/>
+      <c r="R490" s="7"/>
+      <c r="S490" s="6"/>
+      <c r="T490" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U490" s="6"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>993</v>
+        <v>988</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>994</v>
+        <v>989</v>
       </c>
       <c r="C491" s="5">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D491" s="5" t="s">
         <v>811</v>
@@ -31203,7 +31218,7 @@
         <v>24</v>
       </c>
       <c r="F491" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G491" s="6">
         <v>0</v>
@@ -31213,7 +31228,7 @@
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K491" s="6">
         <v>0</v>
@@ -31225,7 +31240,9 @@
         <v>30</v>
       </c>
       <c r="N491" s="7"/>
-      <c r="O491" s="6"/>
+      <c r="O491" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="P491" s="10" t="s">
         <v>25</v>
       </c>
@@ -31233,67 +31250,73 @@
       <c r="R491" s="7"/>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U491" s="6"/>
-    </row>
-    <row r="492" spans="1:21" outlineLevel="1">
-      <c r="A492" s="5" t="s">
-        <v>993</v>
-      </c>
-      <c r="B492" s="5" t="s">
-        <v>994</v>
-      </c>
-      <c r="C492" s="5">
+        <v>965</v>
+      </c>
+      <c r="U491" s="6" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="492" spans="1:21">
+      <c r="A492" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B492" s="2" t="s">
+        <v>999</v>
+      </c>
+      <c r="C492" s="2">
         <v>100</v>
       </c>
-      <c r="D492" s="5" t="s">
+      <c r="D492" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E492" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F492" s="6">
-        <v>2</v>
-      </c>
-      <c r="G492" s="6">
+      <c r="E492" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F492" s="2">
         <v>1</v>
       </c>
-      <c r="H492" s="6" t="s">
-        <v>998</v>
-      </c>
-      <c r="I492" s="6"/>
-      <c r="J492" s="6">
-        <v>1</v>
-      </c>
-      <c r="K492" s="6">
-        <v>0</v>
-      </c>
-      <c r="L492" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M492" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N492" s="7"/>
-      <c r="O492" s="6"/>
-      <c r="P492" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q492" s="6"/>
-      <c r="R492" s="7"/>
-      <c r="S492" s="6"/>
-      <c r="T492" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U492" s="6"/>
+      <c r="G492" s="2">
+        <v>0</v>
+      </c>
+      <c r="H492" s="2" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I492" s="2"/>
+      <c r="J492" s="2">
+        <v>8</v>
+      </c>
+      <c r="K492" s="2">
+        <v>4</v>
+      </c>
+      <c r="L492" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M492" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N492" s="3"/>
+      <c r="O492" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P492" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q492" s="2"/>
+      <c r="R492" s="3"/>
+      <c r="S492" s="2">
+        <v>4</v>
+      </c>
+      <c r="T492" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="U492" s="2"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31308,10 +31331,10 @@
         <v>2</v>
       </c>
       <c r="G493" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31335,16 +31358,16 @@
       <c r="R493" s="7"/>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31359,10 +31382,10 @@
         <v>2</v>
       </c>
       <c r="G494" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31386,16 +31409,16 @@
       <c r="R494" s="7"/>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31410,14 +31433,14 @@
         <v>2</v>
       </c>
       <c r="G495" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K495" s="6">
         <v>0</v>
@@ -31429,9 +31452,7 @@
         <v>30</v>
       </c>
       <c r="N495" s="7"/>
-      <c r="O495" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O495" s="6"/>
       <c r="P495" s="10" t="s">
         <v>25</v>
       </c>
@@ -31439,16 +31460,16 @@
       <c r="R495" s="7"/>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31460,17 +31481,17 @@
         <v>24</v>
       </c>
       <c r="F496" s="6">
+        <v>2</v>
+      </c>
+      <c r="G496" s="6">
         <v>3</v>
       </c>
-      <c r="G496" s="6">
-        <v>0</v>
-      </c>
       <c r="H496" s="6" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K496" s="6">
         <v>0</v>
@@ -31482,9 +31503,7 @@
         <v>30</v>
       </c>
       <c r="N496" s="7"/>
-      <c r="O496" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O496" s="6"/>
       <c r="P496" s="10" t="s">
         <v>25</v>
       </c>
@@ -31492,76 +31511,72 @@
       <c r="R496" s="7"/>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="U496" s="6" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="497" spans="1:21">
-      <c r="A497" s="2" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B497" s="2" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C497" s="2">
-        <v>60</v>
-      </c>
-      <c r="D497" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="U496" s="6"/>
+    </row>
+    <row r="497" spans="1:21" outlineLevel="1">
+      <c r="A497" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B497" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="C497" s="5">
+        <v>100</v>
+      </c>
+      <c r="D497" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="E497" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F497" s="2">
-        <v>1</v>
-      </c>
-      <c r="G497" s="2">
-        <v>0</v>
-      </c>
-      <c r="H497" s="2" t="s">
+      <c r="E497" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F497" s="6">
+        <v>2</v>
+      </c>
+      <c r="G497" s="6">
+        <v>4</v>
+      </c>
+      <c r="H497" s="6" t="s">
         <v>1006</v>
       </c>
-      <c r="I497" s="2"/>
-      <c r="J497" s="2">
-        <v>8</v>
-      </c>
-      <c r="K497" s="2">
-        <v>5</v>
-      </c>
-      <c r="L497" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M497" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N497" s="3"/>
-      <c r="O497" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P497" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q497" s="2"/>
-      <c r="R497" s="3"/>
-      <c r="S497" s="2">
-        <v>5</v>
-      </c>
-      <c r="T497" s="2" t="s">
-        <v>1007</v>
-      </c>
-      <c r="U497" s="2"/>
+      <c r="I497" s="6"/>
+      <c r="J497" s="6">
+        <v>4</v>
+      </c>
+      <c r="K497" s="6">
+        <v>0</v>
+      </c>
+      <c r="L497" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M497" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N497" s="7"/>
+      <c r="O497" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P497" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q497" s="6"/>
+      <c r="R497" s="7"/>
+      <c r="S497" s="6"/>
+      <c r="T497" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U497" s="6"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="C498" s="5">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D498" s="5" t="s">
         <v>811</v>
@@ -31570,17 +31585,17 @@
         <v>24</v>
       </c>
       <c r="F498" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G498" s="6">
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K498" s="6">
         <v>0</v>
@@ -31592,7 +31607,9 @@
         <v>30</v>
       </c>
       <c r="N498" s="7"/>
-      <c r="O498" s="6"/>
+      <c r="O498" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="P498" s="10" t="s">
         <v>25</v>
       </c>
@@ -31600,67 +31617,73 @@
       <c r="R498" s="7"/>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U498" s="6"/>
-    </row>
-    <row r="499" spans="1:21" outlineLevel="1">
-      <c r="A499" s="5" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B499" s="5" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C499" s="5">
+        <v>965</v>
+      </c>
+      <c r="U498" s="6" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="499" spans="1:21">
+      <c r="A499" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B499" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C499" s="2">
         <v>60</v>
       </c>
-      <c r="D499" s="5" t="s">
+      <c r="D499" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E499" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F499" s="6">
-        <v>2</v>
-      </c>
-      <c r="G499" s="6">
+      <c r="E499" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F499" s="2">
         <v>1</v>
       </c>
-      <c r="H499" s="6" t="s">
-        <v>1009</v>
-      </c>
-      <c r="I499" s="6"/>
-      <c r="J499" s="6">
-        <v>1</v>
-      </c>
-      <c r="K499" s="6">
-        <v>0</v>
-      </c>
-      <c r="L499" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M499" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N499" s="7"/>
-      <c r="O499" s="6"/>
-      <c r="P499" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q499" s="6"/>
-      <c r="R499" s="7"/>
-      <c r="S499" s="6"/>
-      <c r="T499" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U499" s="6"/>
+      <c r="G499" s="2">
+        <v>0</v>
+      </c>
+      <c r="H499" s="2" t="s">
+        <v>1011</v>
+      </c>
+      <c r="I499" s="2"/>
+      <c r="J499" s="2">
+        <v>8</v>
+      </c>
+      <c r="K499" s="2">
+        <v>5</v>
+      </c>
+      <c r="L499" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M499" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N499" s="3"/>
+      <c r="O499" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P499" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q499" s="2"/>
+      <c r="R499" s="3"/>
+      <c r="S499" s="2">
+        <v>5</v>
+      </c>
+      <c r="T499" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="U499" s="2"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31675,10 +31698,10 @@
         <v>2</v>
       </c>
       <c r="G500" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1010</v>
+        <v>1013</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31702,16 +31725,16 @@
       <c r="R500" s="7"/>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31726,10 +31749,10 @@
         <v>2</v>
       </c>
       <c r="G501" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1011</v>
+        <v>1014</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31753,16 +31776,16 @@
       <c r="R501" s="7"/>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31777,14 +31800,14 @@
         <v>2</v>
       </c>
       <c r="G502" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K502" s="6">
         <v>0</v>
@@ -31796,9 +31819,7 @@
         <v>30</v>
       </c>
       <c r="N502" s="7"/>
-      <c r="O502" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O502" s="6"/>
       <c r="P502" s="10" t="s">
         <v>25</v>
       </c>
@@ -31806,16 +31827,16 @@
       <c r="R502" s="7"/>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1004</v>
+        <v>1009</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1005</v>
+        <v>1010</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31827,17 +31848,17 @@
         <v>24</v>
       </c>
       <c r="F503" s="6">
+        <v>2</v>
+      </c>
+      <c r="G503" s="6">
         <v>3</v>
       </c>
-      <c r="G503" s="6">
-        <v>0</v>
-      </c>
       <c r="H503" s="6" t="s">
-        <v>1013</v>
+        <v>1016</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K503" s="6">
         <v>0</v>
@@ -31849,9 +31870,7 @@
         <v>30</v>
       </c>
       <c r="N503" s="7"/>
-      <c r="O503" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O503" s="6"/>
       <c r="P503" s="10" t="s">
         <v>25</v>
       </c>
@@ -31859,76 +31878,72 @@
       <c r="R503" s="7"/>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="U503" s="6" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="504" spans="1:21">
-      <c r="A504" s="2" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B504" s="2" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C504" s="2">
-        <v>100</v>
-      </c>
-      <c r="D504" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="U503" s="6"/>
+    </row>
+    <row r="504" spans="1:21" outlineLevel="1">
+      <c r="A504" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B504" s="5" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C504" s="5">
+        <v>60</v>
+      </c>
+      <c r="D504" s="5" t="s">
         <v>811</v>
       </c>
-      <c r="E504" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F504" s="2">
-        <v>1</v>
-      </c>
-      <c r="G504" s="2">
-        <v>0</v>
-      </c>
-      <c r="H504" s="2" t="s">
+      <c r="E504" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F504" s="6">
+        <v>2</v>
+      </c>
+      <c r="G504" s="6">
+        <v>4</v>
+      </c>
+      <c r="H504" s="6" t="s">
         <v>1017</v>
       </c>
-      <c r="I504" s="2"/>
-      <c r="J504" s="2">
-        <v>8</v>
-      </c>
-      <c r="K504" s="2">
-        <v>6</v>
-      </c>
-      <c r="L504" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M504" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N504" s="3"/>
-      <c r="O504" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P504" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q504" s="2"/>
-      <c r="R504" s="3"/>
-      <c r="S504" s="2">
-        <v>6</v>
-      </c>
-      <c r="T504" s="2" t="s">
-        <v>1018</v>
-      </c>
-      <c r="U504" s="2"/>
+      <c r="I504" s="6"/>
+      <c r="J504" s="6">
+        <v>4</v>
+      </c>
+      <c r="K504" s="6">
+        <v>0</v>
+      </c>
+      <c r="L504" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M504" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N504" s="7"/>
+      <c r="O504" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P504" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q504" s="6"/>
+      <c r="R504" s="7"/>
+      <c r="S504" s="6"/>
+      <c r="T504" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U504" s="6"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="C505" s="5">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D505" s="5" t="s">
         <v>811</v>
@@ -31937,17 +31952,17 @@
         <v>24</v>
       </c>
       <c r="F505" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G505" s="6">
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K505" s="6">
         <v>0</v>
@@ -31959,7 +31974,9 @@
         <v>30</v>
       </c>
       <c r="N505" s="7"/>
-      <c r="O505" s="6"/>
+      <c r="O505" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="P505" s="10" t="s">
         <v>25</v>
       </c>
@@ -31967,67 +31984,73 @@
       <c r="R505" s="7"/>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U505" s="6"/>
-    </row>
-    <row r="506" spans="1:21" outlineLevel="1">
-      <c r="A506" s="5" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B506" s="5" t="s">
-        <v>1016</v>
-      </c>
-      <c r="C506" s="5">
+        <v>965</v>
+      </c>
+      <c r="U505" s="6" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="506" spans="1:21">
+      <c r="A506" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C506" s="2">
         <v>100</v>
       </c>
-      <c r="D506" s="5" t="s">
+      <c r="D506" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E506" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F506" s="6">
-        <v>2</v>
-      </c>
-      <c r="G506" s="6">
+      <c r="E506" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F506" s="2">
         <v>1</v>
       </c>
-      <c r="H506" s="6" t="s">
-        <v>1020</v>
-      </c>
-      <c r="I506" s="6"/>
-      <c r="J506" s="6">
-        <v>1</v>
-      </c>
-      <c r="K506" s="6">
-        <v>0</v>
-      </c>
-      <c r="L506" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M506" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N506" s="7"/>
-      <c r="O506" s="6"/>
-      <c r="P506" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q506" s="6"/>
-      <c r="R506" s="7"/>
-      <c r="S506" s="6"/>
-      <c r="T506" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U506" s="6"/>
+      <c r="G506" s="2">
+        <v>0</v>
+      </c>
+      <c r="H506" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="I506" s="2"/>
+      <c r="J506" s="2">
+        <v>8</v>
+      </c>
+      <c r="K506" s="2">
+        <v>6</v>
+      </c>
+      <c r="L506" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M506" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N506" s="3"/>
+      <c r="O506" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P506" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q506" s="2"/>
+      <c r="R506" s="3"/>
+      <c r="S506" s="2">
+        <v>6</v>
+      </c>
+      <c r="T506" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="U506" s="2"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32042,10 +32065,10 @@
         <v>2</v>
       </c>
       <c r="G507" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32069,16 +32092,16 @@
       <c r="R507" s="7"/>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32093,10 +32116,10 @@
         <v>2</v>
       </c>
       <c r="G508" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32120,16 +32143,16 @@
       <c r="R508" s="7"/>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32144,14 +32167,14 @@
         <v>2</v>
       </c>
       <c r="G509" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K509" s="6">
         <v>0</v>
@@ -32163,9 +32186,7 @@
         <v>30</v>
       </c>
       <c r="N509" s="7"/>
-      <c r="O509" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O509" s="6"/>
       <c r="P509" s="10" t="s">
         <v>25</v>
       </c>
@@ -32173,16 +32194,16 @@
       <c r="R509" s="7"/>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1015</v>
+        <v>1020</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32194,17 +32215,17 @@
         <v>24</v>
       </c>
       <c r="F510" s="6">
+        <v>2</v>
+      </c>
+      <c r="G510" s="6">
         <v>3</v>
       </c>
-      <c r="G510" s="6">
-        <v>0</v>
-      </c>
       <c r="H510" s="6" t="s">
-        <v>1024</v>
+        <v>1027</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K510" s="6">
         <v>0</v>
@@ -32216,9 +32237,7 @@
         <v>30</v>
       </c>
       <c r="N510" s="7"/>
-      <c r="O510" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O510" s="6"/>
       <c r="P510" s="10" t="s">
         <v>25</v>
       </c>
@@ -32226,73 +32245,69 @@
       <c r="R510" s="7"/>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>1025</v>
-      </c>
-      <c r="U510" s="6" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="511" spans="1:21">
-      <c r="A511" s="2" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B511" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="U510" s="6"/>
+    </row>
+    <row r="511" spans="1:21" outlineLevel="1">
+      <c r="A511" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B511" s="5" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C511" s="5">
+        <v>100</v>
+      </c>
+      <c r="D511" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E511" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F511" s="6">
+        <v>2</v>
+      </c>
+      <c r="G511" s="6">
+        <v>4</v>
+      </c>
+      <c r="H511" s="6" t="s">
         <v>1028</v>
       </c>
-      <c r="C511" s="2">
-        <v>100</v>
-      </c>
-      <c r="D511" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="E511" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F511" s="2">
-        <v>1</v>
-      </c>
-      <c r="G511" s="2">
-        <v>0</v>
-      </c>
-      <c r="H511" s="2" t="s">
-        <v>1029</v>
-      </c>
-      <c r="I511" s="2"/>
-      <c r="J511" s="2">
-        <v>8</v>
-      </c>
-      <c r="K511" s="2">
-        <v>7</v>
-      </c>
-      <c r="L511" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M511" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N511" s="3"/>
-      <c r="O511" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P511" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q511" s="2"/>
-      <c r="R511" s="3"/>
-      <c r="S511" s="2">
-        <v>7</v>
-      </c>
-      <c r="T511" s="2" t="s">
-        <v>1030</v>
-      </c>
-      <c r="U511" s="2"/>
+      <c r="I511" s="6"/>
+      <c r="J511" s="6">
+        <v>4</v>
+      </c>
+      <c r="K511" s="6">
+        <v>0</v>
+      </c>
+      <c r="L511" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M511" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N511" s="7"/>
+      <c r="O511" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P511" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q511" s="6"/>
+      <c r="R511" s="7"/>
+      <c r="S511" s="6"/>
+      <c r="T511" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U511" s="6"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1027</v>
+        <v>1020</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1028</v>
+        <v>1021</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32304,17 +32319,17 @@
         <v>24</v>
       </c>
       <c r="F512" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G512" s="6">
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="K512" s="6">
         <v>0</v>
@@ -32326,7 +32341,9 @@
         <v>30</v>
       </c>
       <c r="N512" s="7"/>
-      <c r="O512" s="6"/>
+      <c r="O512" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="P512" s="10" t="s">
         <v>25</v>
       </c>
@@ -32334,67 +32351,73 @@
       <c r="R512" s="7"/>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U512" s="6"/>
-    </row>
-    <row r="513" spans="1:21" outlineLevel="1">
-      <c r="A513" s="5" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B513" s="5" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C513" s="5">
+        <v>1030</v>
+      </c>
+      <c r="U512" s="6" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="513" spans="1:21">
+      <c r="A513" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B513" s="2" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C513" s="2">
         <v>100</v>
       </c>
-      <c r="D513" s="5" t="s">
+      <c r="D513" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E513" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F513" s="6">
-        <v>2</v>
-      </c>
-      <c r="G513" s="6">
+      <c r="E513" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F513" s="2">
         <v>1</v>
       </c>
-      <c r="H513" s="6" t="s">
-        <v>1032</v>
-      </c>
-      <c r="I513" s="6"/>
-      <c r="J513" s="6">
-        <v>1</v>
-      </c>
-      <c r="K513" s="6">
-        <v>0</v>
-      </c>
-      <c r="L513" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M513" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N513" s="7"/>
-      <c r="O513" s="6"/>
-      <c r="P513" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q513" s="6"/>
-      <c r="R513" s="7"/>
-      <c r="S513" s="6"/>
-      <c r="T513" s="6" t="s">
-        <v>954</v>
-      </c>
-      <c r="U513" s="6"/>
+      <c r="G513" s="2">
+        <v>0</v>
+      </c>
+      <c r="H513" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I513" s="2"/>
+      <c r="J513" s="2">
+        <v>8</v>
+      </c>
+      <c r="K513" s="2">
+        <v>7</v>
+      </c>
+      <c r="L513" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M513" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N513" s="3"/>
+      <c r="O513" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P513" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q513" s="2"/>
+      <c r="R513" s="3"/>
+      <c r="S513" s="2">
+        <v>7</v>
+      </c>
+      <c r="T513" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="U513" s="2"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1027</v>
+        <v>1032</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32409,10 +32432,10 @@
         <v>2</v>
       </c>
       <c r="G514" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1033</v>
+        <v>1036</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32436,16 +32459,16 @@
       <c r="R514" s="7"/>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1027</v>
+        <v>1032</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32460,10 +32483,10 @@
         <v>2</v>
       </c>
       <c r="G515" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32487,16 +32510,16 @@
       <c r="R515" s="7"/>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1027</v>
+        <v>1032</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32511,14 +32534,14 @@
         <v>2</v>
       </c>
       <c r="G516" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K516" s="6">
         <v>0</v>
@@ -32530,9 +32553,7 @@
         <v>30</v>
       </c>
       <c r="N516" s="7"/>
-      <c r="O516" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O516" s="6"/>
       <c r="P516" s="10" t="s">
         <v>25</v>
       </c>
@@ -32540,16 +32561,16 @@
       <c r="R516" s="7"/>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>954</v>
+        <v>959</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1027</v>
+        <v>1032</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1028</v>
+        <v>1033</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32561,17 +32582,17 @@
         <v>24</v>
       </c>
       <c r="F517" s="6">
+        <v>2</v>
+      </c>
+      <c r="G517" s="6">
         <v>3</v>
       </c>
-      <c r="G517" s="6">
-        <v>0</v>
-      </c>
       <c r="H517" s="6" t="s">
-        <v>1036</v>
+        <v>1039</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="K517" s="6">
         <v>0</v>
@@ -32583,9 +32604,7 @@
         <v>30</v>
       </c>
       <c r="N517" s="7"/>
-      <c r="O517" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="O517" s="6"/>
       <c r="P517" s="10" t="s">
         <v>25</v>
       </c>
@@ -32593,14 +32612,120 @@
       <c r="R517" s="7"/>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
-      </c>
-      <c r="U517" s="6" t="s">
-        <v>1037</v>
+        <v>959</v>
+      </c>
+      <c r="U517" s="6"/>
+    </row>
+    <row r="518" spans="1:21" outlineLevel="1">
+      <c r="A518" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B518" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C518" s="5">
+        <v>100</v>
+      </c>
+      <c r="D518" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E518" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F518" s="6">
+        <v>2</v>
+      </c>
+      <c r="G518" s="6">
+        <v>4</v>
+      </c>
+      <c r="H518" s="6" t="s">
+        <v>1040</v>
+      </c>
+      <c r="I518" s="6"/>
+      <c r="J518" s="6">
+        <v>4</v>
+      </c>
+      <c r="K518" s="6">
+        <v>0</v>
+      </c>
+      <c r="L518" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M518" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N518" s="7"/>
+      <c r="O518" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P518" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q518" s="6"/>
+      <c r="R518" s="7"/>
+      <c r="S518" s="6"/>
+      <c r="T518" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="U518" s="6"/>
+    </row>
+    <row r="519" spans="1:21" outlineLevel="1">
+      <c r="A519" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B519" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C519" s="5">
+        <v>100</v>
+      </c>
+      <c r="D519" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E519" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F519" s="6">
+        <v>3</v>
+      </c>
+      <c r="G519" s="6">
+        <v>0</v>
+      </c>
+      <c r="H519" s="6" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I519" s="6"/>
+      <c r="J519" s="6">
+        <v>32</v>
+      </c>
+      <c r="K519" s="6">
+        <v>0</v>
+      </c>
+      <c r="L519" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M519" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N519" s="7"/>
+      <c r="O519" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P519" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q519" s="6"/>
+      <c r="R519" s="7"/>
+      <c r="S519" s="6"/>
+      <c r="T519" s="6" t="s">
+        <v>965</v>
+      </c>
+      <c r="U519" s="6" t="s">
+        <v>1042</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD518"/>
+  <autoFilter ref="A1:AD520"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at 463e35d
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5998" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5998" uniqueCount="1044">
   <si>
     <t>ID</t>
   </si>
@@ -2816,6 +2816,9 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
+  </si>
+  <si>
+    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29246,7 +29249,7 @@
         <v>0</v>
       </c>
       <c r="T453" s="2" t="s">
-        <v>863</v>
+        <v>933</v>
       </c>
       <c r="U453" s="2"/>
     </row>
@@ -29305,7 +29308,7 @@
         <v>1</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29364,7 +29367,7 @@
         <v>2</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29423,7 +29426,7 @@
         <v>3</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29482,7 +29485,7 @@
         <v>4</v>
       </c>
       <c r="T457" s="6" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="U457" s="5"/>
     </row>
@@ -29541,7 +29544,7 @@
         <v>6</v>
       </c>
       <c r="T458" s="6" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="U458" s="5"/>
     </row>
@@ -29568,10 +29571,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="I459" s="6" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>16</v>
@@ -29598,18 +29601,18 @@
       </c>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="U459" s="6" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C460" s="2">
         <v>1000</v>
@@ -29627,10 +29630,10 @@
         <v>0</v>
       </c>
       <c r="H460" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="I460" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="J460" s="2">
         <v>32</v>
@@ -29657,16 +29660,16 @@
       </c>
       <c r="S460" s="2"/>
       <c r="T460" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="U460" s="2"/>
     </row>
     <row r="461" spans="1:21" outlineLevel="1">
       <c r="A461" s="5" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B461" s="5" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C461" s="5">
         <v>1000</v>
@@ -29684,10 +29687,10 @@
         <v>0</v>
       </c>
       <c r="H461" s="6" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="I461" s="6" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="J461" s="6">
         <v>32</v>
@@ -29714,22 +29717,22 @@
       </c>
       <c r="S461" s="6"/>
       <c r="T461" s="6" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="U461" s="6"/>
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C462" s="2">
         <v>0</v>
       </c>
       <c r="D462" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="E462" s="2" t="s">
         <v>24</v>
@@ -29755,16 +29758,16 @@
     </row>
     <row r="463" spans="1:21">
       <c r="A463" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B463" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="C463" s="2">
         <v>0</v>
       </c>
       <c r="D463" s="2" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="E463" s="2" t="s">
         <v>24</v>
@@ -29790,10 +29793,10 @@
     </row>
     <row r="464" spans="1:21">
       <c r="A464" s="2" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C464" s="2">
         <v>20</v>
@@ -29811,7 +29814,7 @@
         <v>0</v>
       </c>
       <c r="H464" s="2" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="I464" s="2"/>
       <c r="J464" s="2">
@@ -29839,16 +29842,16 @@
         <v>0</v>
       </c>
       <c r="T464" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="U464" s="2"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B465" s="5" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29866,7 +29869,7 @@
         <v>0</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29890,16 +29893,16 @@
       <c r="R465" s="7"/>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B466" s="5" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29917,7 +29920,7 @@
         <v>1</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29941,16 +29944,16 @@
       <c r="R466" s="7"/>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B467" s="5" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29968,7 +29971,7 @@
         <v>2</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29992,16 +29995,16 @@
       <c r="R467" s="7"/>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B468" s="5" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -30019,7 +30022,7 @@
         <v>3</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30043,16 +30046,16 @@
       <c r="R468" s="7"/>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U468" s="6"/>
     </row>
     <row r="469" spans="1:21" outlineLevel="1">
       <c r="A469" s="5" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B469" s="5" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C469" s="5">
         <v>20</v>
@@ -30070,7 +30073,7 @@
         <v>4</v>
       </c>
       <c r="H469" s="6" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="I469" s="6"/>
       <c r="J469" s="6">
@@ -30096,16 +30099,16 @@
       <c r="R469" s="7"/>
       <c r="S469" s="6"/>
       <c r="T469" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U469" s="6"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B470" s="5" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="C470" s="5">
         <v>20</v>
@@ -30123,7 +30126,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30149,18 +30152,18 @@
       <c r="R470" s="7"/>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U470" s="6" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="471" spans="1:21">
       <c r="A471" s="2" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B471" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C471" s="2">
         <v>60</v>
@@ -30178,7 +30181,7 @@
         <v>0</v>
       </c>
       <c r="H471" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="I471" s="2"/>
       <c r="J471" s="2">
@@ -30206,16 +30209,16 @@
         <v>1</v>
       </c>
       <c r="T471" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="U471" s="2"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B472" s="5" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30233,7 +30236,7 @@
         <v>0</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30257,16 +30260,16 @@
       <c r="R472" s="7"/>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B473" s="5" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30284,7 +30287,7 @@
         <v>1</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30308,16 +30311,16 @@
       <c r="R473" s="7"/>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B474" s="5" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30335,7 +30338,7 @@
         <v>2</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30359,16 +30362,16 @@
       <c r="R474" s="7"/>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B475" s="5" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30386,7 +30389,7 @@
         <v>3</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30410,16 +30413,16 @@
       <c r="R475" s="7"/>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U475" s="6"/>
     </row>
     <row r="476" spans="1:21" outlineLevel="1">
       <c r="A476" s="5" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B476" s="5" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C476" s="5">
         <v>60</v>
@@ -30437,7 +30440,7 @@
         <v>4</v>
       </c>
       <c r="H476" s="6" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="I476" s="6"/>
       <c r="J476" s="6">
@@ -30463,16 +30466,16 @@
       <c r="R476" s="7"/>
       <c r="S476" s="6"/>
       <c r="T476" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U476" s="6"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="B477" s="5" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30490,7 +30493,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30516,18 +30519,18 @@
       <c r="R477" s="7"/>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U477" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="478" spans="1:21">
       <c r="A478" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C478" s="2">
         <v>60</v>
@@ -30545,7 +30548,7 @@
         <v>0</v>
       </c>
       <c r="H478" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="I478" s="2"/>
       <c r="J478" s="2">
@@ -30573,16 +30576,16 @@
         <v>2</v>
       </c>
       <c r="T478" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="U478" s="2"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B479" s="5" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30600,7 +30603,7 @@
         <v>0</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30624,16 +30627,16 @@
       <c r="R479" s="7"/>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B480" s="5" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30651,7 +30654,7 @@
         <v>1</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30675,16 +30678,16 @@
       <c r="R480" s="7"/>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B481" s="5" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30702,7 +30705,7 @@
         <v>2</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30726,16 +30729,16 @@
       <c r="R481" s="7"/>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B482" s="5" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30753,7 +30756,7 @@
         <v>3</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30777,16 +30780,16 @@
       <c r="R482" s="7"/>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U482" s="6"/>
     </row>
     <row r="483" spans="1:21" outlineLevel="1">
       <c r="A483" s="5" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B483" s="5" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C483" s="5">
         <v>60</v>
@@ -30804,7 +30807,7 @@
         <v>4</v>
       </c>
       <c r="H483" s="6" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="I483" s="6"/>
       <c r="J483" s="6">
@@ -30830,16 +30833,16 @@
       <c r="R483" s="7"/>
       <c r="S483" s="6"/>
       <c r="T483" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U483" s="6"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="B484" s="5" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30857,7 +30860,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30883,18 +30886,18 @@
       <c r="R484" s="7"/>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U484" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="485" spans="1:21">
       <c r="A485" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B485" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C485" s="2">
         <v>60</v>
@@ -30912,7 +30915,7 @@
         <v>0</v>
       </c>
       <c r="H485" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="I485" s="2"/>
       <c r="J485" s="2">
@@ -30940,16 +30943,16 @@
         <v>3</v>
       </c>
       <c r="T485" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="U485" s="2"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B486" s="5" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30967,7 +30970,7 @@
         <v>0</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30991,16 +30994,16 @@
       <c r="R486" s="7"/>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -31018,7 +31021,7 @@
         <v>1</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31042,16 +31045,16 @@
       <c r="R487" s="7"/>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B488" s="5" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31069,7 +31072,7 @@
         <v>2</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31093,16 +31096,16 @@
       <c r="R488" s="7"/>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B489" s="5" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31120,7 +31123,7 @@
         <v>3</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31144,16 +31147,16 @@
       <c r="R489" s="7"/>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U489" s="6"/>
     </row>
     <row r="490" spans="1:21" outlineLevel="1">
       <c r="A490" s="5" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B490" s="5" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C490" s="5">
         <v>60</v>
@@ -31171,7 +31174,7 @@
         <v>4</v>
       </c>
       <c r="H490" s="6" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="I490" s="6"/>
       <c r="J490" s="6">
@@ -31197,16 +31200,16 @@
       <c r="R490" s="7"/>
       <c r="S490" s="6"/>
       <c r="T490" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U490" s="6"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B491" s="5" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C491" s="5">
         <v>60</v>
@@ -31224,7 +31227,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31250,18 +31253,18 @@
       <c r="R491" s="7"/>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U491" s="6" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="492" spans="1:21">
       <c r="A492" s="2" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C492" s="2">
         <v>100</v>
@@ -31279,7 +31282,7 @@
         <v>0</v>
       </c>
       <c r="H492" s="2" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I492" s="2"/>
       <c r="J492" s="2">
@@ -31307,16 +31310,16 @@
         <v>4</v>
       </c>
       <c r="T492" s="2" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="U492" s="2"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B493" s="5" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31334,7 +31337,7 @@
         <v>0</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31358,16 +31361,16 @@
       <c r="R493" s="7"/>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B494" s="5" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31385,7 +31388,7 @@
         <v>1</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31409,16 +31412,16 @@
       <c r="R494" s="7"/>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B495" s="5" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31436,7 +31439,7 @@
         <v>2</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31460,16 +31463,16 @@
       <c r="R495" s="7"/>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B496" s="5" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31487,7 +31490,7 @@
         <v>3</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31511,16 +31514,16 @@
       <c r="R496" s="7"/>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U496" s="6"/>
     </row>
     <row r="497" spans="1:21" outlineLevel="1">
       <c r="A497" s="5" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B497" s="5" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C497" s="5">
         <v>100</v>
@@ -31538,7 +31541,7 @@
         <v>4</v>
       </c>
       <c r="H497" s="6" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="I497" s="6"/>
       <c r="J497" s="6">
@@ -31564,16 +31567,16 @@
       <c r="R497" s="7"/>
       <c r="S497" s="6"/>
       <c r="T497" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U497" s="6"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="B498" s="5" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="C498" s="5">
         <v>100</v>
@@ -31591,7 +31594,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31617,18 +31620,18 @@
       <c r="R498" s="7"/>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U498" s="6" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="499" spans="1:21">
       <c r="A499" s="2" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C499" s="2">
         <v>60</v>
@@ -31646,7 +31649,7 @@
         <v>0</v>
       </c>
       <c r="H499" s="2" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="I499" s="2"/>
       <c r="J499" s="2">
@@ -31674,16 +31677,16 @@
         <v>5</v>
       </c>
       <c r="T499" s="2" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="U499" s="2"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B500" s="5" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31701,7 +31704,7 @@
         <v>0</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31725,16 +31728,16 @@
       <c r="R500" s="7"/>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B501" s="5" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31752,7 +31755,7 @@
         <v>1</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31776,16 +31779,16 @@
       <c r="R501" s="7"/>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B502" s="5" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31803,7 +31806,7 @@
         <v>2</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31827,16 +31830,16 @@
       <c r="R502" s="7"/>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31854,7 +31857,7 @@
         <v>3</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31878,16 +31881,16 @@
       <c r="R503" s="7"/>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U503" s="6"/>
     </row>
     <row r="504" spans="1:21" outlineLevel="1">
       <c r="A504" s="5" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B504" s="5" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C504" s="5">
         <v>60</v>
@@ -31905,7 +31908,7 @@
         <v>4</v>
       </c>
       <c r="H504" s="6" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="I504" s="6"/>
       <c r="J504" s="6">
@@ -31931,16 +31934,16 @@
       <c r="R504" s="7"/>
       <c r="S504" s="6"/>
       <c r="T504" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U504" s="6"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B505" s="5" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C505" s="5">
         <v>60</v>
@@ -31958,7 +31961,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31984,18 +31987,18 @@
       <c r="R505" s="7"/>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U505" s="6" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="506" spans="1:21">
       <c r="A506" s="2" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B506" s="2" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C506" s="2">
         <v>100</v>
@@ -32013,7 +32016,7 @@
         <v>0</v>
       </c>
       <c r="H506" s="2" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="I506" s="2"/>
       <c r="J506" s="2">
@@ -32041,16 +32044,16 @@
         <v>6</v>
       </c>
       <c r="T506" s="2" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="U506" s="2"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B507" s="5" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32068,7 +32071,7 @@
         <v>0</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32092,16 +32095,16 @@
       <c r="R507" s="7"/>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B508" s="5" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32119,7 +32122,7 @@
         <v>1</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32143,16 +32146,16 @@
       <c r="R508" s="7"/>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B509" s="5" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32170,7 +32173,7 @@
         <v>2</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32194,16 +32197,16 @@
       <c r="R509" s="7"/>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B510" s="5" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32221,7 +32224,7 @@
         <v>3</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32245,16 +32248,16 @@
       <c r="R510" s="7"/>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U510" s="6"/>
     </row>
     <row r="511" spans="1:21" outlineLevel="1">
       <c r="A511" s="5" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B511" s="5" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C511" s="5">
         <v>100</v>
@@ -32272,7 +32275,7 @@
         <v>4</v>
       </c>
       <c r="H511" s="6" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="I511" s="6"/>
       <c r="J511" s="6">
@@ -32298,16 +32301,16 @@
       <c r="R511" s="7"/>
       <c r="S511" s="6"/>
       <c r="T511" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U511" s="6"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B512" s="5" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32325,7 +32328,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32351,18 +32354,18 @@
       <c r="R512" s="7"/>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="U512" s="6" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="513" spans="1:21">
       <c r="A513" s="2" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B513" s="2" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C513" s="2">
         <v>100</v>
@@ -32380,7 +32383,7 @@
         <v>0</v>
       </c>
       <c r="H513" s="2" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="I513" s="2"/>
       <c r="J513" s="2">
@@ -32408,16 +32411,16 @@
         <v>7</v>
       </c>
       <c r="T513" s="2" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="U513" s="2"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B514" s="5" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32435,7 +32438,7 @@
         <v>0</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32459,16 +32462,16 @@
       <c r="R514" s="7"/>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B515" s="5" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32486,7 +32489,7 @@
         <v>1</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32510,16 +32513,16 @@
       <c r="R515" s="7"/>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B516" s="5" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32537,7 +32540,7 @@
         <v>2</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32561,16 +32564,16 @@
       <c r="R516" s="7"/>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B517" s="5" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32588,7 +32591,7 @@
         <v>3</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32612,16 +32615,16 @@
       <c r="R517" s="7"/>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U517" s="6"/>
     </row>
     <row r="518" spans="1:21" outlineLevel="1">
       <c r="A518" s="5" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B518" s="5" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C518" s="5">
         <v>100</v>
@@ -32639,7 +32642,7 @@
         <v>4</v>
       </c>
       <c r="H518" s="6" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="I518" s="6"/>
       <c r="J518" s="6">
@@ -32665,16 +32668,16 @@
       <c r="R518" s="7"/>
       <c r="S518" s="6"/>
       <c r="T518" s="6" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="U518" s="6"/>
     </row>
     <row r="519" spans="1:21" outlineLevel="1">
       <c r="A519" s="5" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B519" s="5" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="C519" s="5">
         <v>100</v>
@@ -32692,7 +32695,7 @@
         <v>0</v>
       </c>
       <c r="H519" s="6" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="I519" s="6"/>
       <c r="J519" s="6">
@@ -32718,10 +32721,10 @@
       <c r="R519" s="7"/>
       <c r="S519" s="6"/>
       <c r="T519" s="6" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="U519" s="6" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at 38f9c6c
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5998" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5998" uniqueCount="1043">
   <si>
     <t>ID</t>
   </si>
@@ -2816,9 +2816,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29249,7 +29246,7 @@
         <v>0</v>
       </c>
       <c r="T453" s="2" t="s">
-        <v>933</v>
+        <v>863</v>
       </c>
       <c r="U453" s="2"/>
     </row>
@@ -29308,7 +29305,7 @@
         <v>1</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29367,7 +29364,7 @@
         <v>2</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29426,7 +29423,7 @@
         <v>3</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29485,7 +29482,7 @@
         <v>4</v>
       </c>
       <c r="T457" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="U457" s="5"/>
     </row>
@@ -29544,7 +29541,7 @@
         <v>6</v>
       </c>
       <c r="T458" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="U458" s="5"/>
     </row>
@@ -29571,10 +29568,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
+        <v>938</v>
+      </c>
+      <c r="I459" s="6" t="s">
         <v>939</v>
-      </c>
-      <c r="I459" s="6" t="s">
-        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>16</v>
@@ -29601,18 +29598,18 @@
       </c>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="U459" s="6" t="s">
         <v>941</v>
-      </c>
-      <c r="U459" s="6" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>943</v>
-      </c>
-      <c r="B460" s="2" t="s">
-        <v>944</v>
       </c>
       <c r="C460" s="2">
         <v>1000</v>
@@ -29630,10 +29627,10 @@
         <v>0</v>
       </c>
       <c r="H460" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="I460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="I460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="J460" s="2">
         <v>32</v>
@@ -29660,16 +29657,16 @@
       </c>
       <c r="S460" s="2"/>
       <c r="T460" s="2" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="U460" s="2"/>
     </row>
     <row r="461" spans="1:21" outlineLevel="1">
       <c r="A461" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="B461" s="5" t="s">
         <v>943</v>
-      </c>
-      <c r="B461" s="5" t="s">
-        <v>944</v>
       </c>
       <c r="C461" s="5">
         <v>1000</v>
@@ -29687,10 +29684,10 @@
         <v>0</v>
       </c>
       <c r="H461" s="6" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="I461" s="6" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="J461" s="6">
         <v>32</v>
@@ -29717,22 +29714,22 @@
       </c>
       <c r="S461" s="6"/>
       <c r="T461" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="U461" s="6"/>
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>949</v>
       </c>
-      <c r="B462" s="2" t="s">
+      <c r="C462" s="2">
+        <v>0</v>
+      </c>
+      <c r="D462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="C462" s="2">
-        <v>0</v>
-      </c>
-      <c r="D462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="E462" s="2" t="s">
         <v>24</v>
@@ -29758,16 +29755,16 @@
     </row>
     <row r="463" spans="1:21">
       <c r="A463" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="B463" s="2" t="s">
         <v>952</v>
       </c>
-      <c r="B463" s="2" t="s">
+      <c r="C463" s="2">
+        <v>0</v>
+      </c>
+      <c r="D463" s="2" t="s">
         <v>953</v>
-      </c>
-      <c r="C463" s="2">
-        <v>0</v>
-      </c>
-      <c r="D463" s="2" t="s">
-        <v>954</v>
       </c>
       <c r="E463" s="2" t="s">
         <v>24</v>
@@ -29793,10 +29790,10 @@
     </row>
     <row r="464" spans="1:21">
       <c r="A464" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B464" s="2" t="s">
         <v>955</v>
-      </c>
-      <c r="B464" s="2" t="s">
-        <v>956</v>
       </c>
       <c r="C464" s="2">
         <v>20</v>
@@ -29814,7 +29811,7 @@
         <v>0</v>
       </c>
       <c r="H464" s="2" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I464" s="2"/>
       <c r="J464" s="2">
@@ -29842,16 +29839,16 @@
         <v>0</v>
       </c>
       <c r="T464" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="U464" s="2"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29869,7 +29866,7 @@
         <v>0</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29893,16 +29890,16 @@
       <c r="R465" s="7"/>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29920,7 +29917,7 @@
         <v>1</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29944,16 +29941,16 @@
       <c r="R466" s="7"/>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29971,7 +29968,7 @@
         <v>2</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29995,16 +29992,16 @@
       <c r="R467" s="7"/>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -30022,7 +30019,7 @@
         <v>3</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30046,16 +30043,16 @@
       <c r="R468" s="7"/>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U468" s="6"/>
     </row>
     <row r="469" spans="1:21" outlineLevel="1">
       <c r="A469" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B469" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B469" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C469" s="5">
         <v>20</v>
@@ -30073,7 +30070,7 @@
         <v>4</v>
       </c>
       <c r="H469" s="6" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I469" s="6"/>
       <c r="J469" s="6">
@@ -30099,16 +30096,16 @@
       <c r="R469" s="7"/>
       <c r="S469" s="6"/>
       <c r="T469" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U469" s="6"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C470" s="5">
         <v>20</v>
@@ -30126,7 +30123,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30152,18 +30149,18 @@
       <c r="R470" s="7"/>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
+        <v>965</v>
+      </c>
+      <c r="U470" s="6" t="s">
         <v>966</v>
-      </c>
-      <c r="U470" s="6" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="471" spans="1:21">
       <c r="A471" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B471" s="2" t="s">
         <v>968</v>
-      </c>
-      <c r="B471" s="2" t="s">
-        <v>969</v>
       </c>
       <c r="C471" s="2">
         <v>60</v>
@@ -30181,7 +30178,7 @@
         <v>0</v>
       </c>
       <c r="H471" s="2" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I471" s="2"/>
       <c r="J471" s="2">
@@ -30209,16 +30206,16 @@
         <v>1</v>
       </c>
       <c r="T471" s="2" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="U471" s="2"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30236,7 +30233,7 @@
         <v>0</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30260,16 +30257,16 @@
       <c r="R472" s="7"/>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30287,7 +30284,7 @@
         <v>1</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30311,16 +30308,16 @@
       <c r="R473" s="7"/>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30338,7 +30335,7 @@
         <v>2</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30362,16 +30359,16 @@
       <c r="R474" s="7"/>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30389,7 +30386,7 @@
         <v>3</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30413,16 +30410,16 @@
       <c r="R475" s="7"/>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U475" s="6"/>
     </row>
     <row r="476" spans="1:21" outlineLevel="1">
       <c r="A476" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B476" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B476" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C476" s="5">
         <v>60</v>
@@ -30440,7 +30437,7 @@
         <v>4</v>
       </c>
       <c r="H476" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="6"/>
       <c r="J476" s="6">
@@ -30466,16 +30463,16 @@
       <c r="R476" s="7"/>
       <c r="S476" s="6"/>
       <c r="T476" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U476" s="6"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30493,7 +30490,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30519,18 +30516,18 @@
       <c r="R477" s="7"/>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="478" spans="1:21">
       <c r="A478" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B478" s="2" t="s">
         <v>979</v>
-      </c>
-      <c r="B478" s="2" t="s">
-        <v>980</v>
       </c>
       <c r="C478" s="2">
         <v>60</v>
@@ -30548,7 +30545,7 @@
         <v>0</v>
       </c>
       <c r="H478" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I478" s="2"/>
       <c r="J478" s="2">
@@ -30576,16 +30573,16 @@
         <v>2</v>
       </c>
       <c r="T478" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="U478" s="2"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30603,7 +30600,7 @@
         <v>0</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30627,16 +30624,16 @@
       <c r="R479" s="7"/>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30654,7 +30651,7 @@
         <v>1</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30678,16 +30675,16 @@
       <c r="R480" s="7"/>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30705,7 +30702,7 @@
         <v>2</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30729,16 +30726,16 @@
       <c r="R481" s="7"/>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30756,7 +30753,7 @@
         <v>3</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30780,16 +30777,16 @@
       <c r="R482" s="7"/>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U482" s="6"/>
     </row>
     <row r="483" spans="1:21" outlineLevel="1">
       <c r="A483" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B483" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B483" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C483" s="5">
         <v>60</v>
@@ -30807,7 +30804,7 @@
         <v>4</v>
       </c>
       <c r="H483" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="I483" s="6"/>
       <c r="J483" s="6">
@@ -30833,16 +30830,16 @@
       <c r="R483" s="7"/>
       <c r="S483" s="6"/>
       <c r="T483" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U483" s="6"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30860,7 +30857,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30886,18 +30883,18 @@
       <c r="R484" s="7"/>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U484" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="485" spans="1:21">
       <c r="A485" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B485" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="B485" s="2" t="s">
-        <v>990</v>
       </c>
       <c r="C485" s="2">
         <v>60</v>
@@ -30915,7 +30912,7 @@
         <v>0</v>
       </c>
       <c r="H485" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I485" s="2"/>
       <c r="J485" s="2">
@@ -30943,16 +30940,16 @@
         <v>3</v>
       </c>
       <c r="T485" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="U485" s="2"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30970,7 +30967,7 @@
         <v>0</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30994,16 +30991,16 @@
       <c r="R486" s="7"/>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -31021,7 +31018,7 @@
         <v>1</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31045,16 +31042,16 @@
       <c r="R487" s="7"/>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31072,7 +31069,7 @@
         <v>2</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31096,16 +31093,16 @@
       <c r="R488" s="7"/>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31123,7 +31120,7 @@
         <v>3</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31147,16 +31144,16 @@
       <c r="R489" s="7"/>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U489" s="6"/>
     </row>
     <row r="490" spans="1:21" outlineLevel="1">
       <c r="A490" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B490" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B490" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C490" s="5">
         <v>60</v>
@@ -31174,7 +31171,7 @@
         <v>4</v>
       </c>
       <c r="H490" s="6" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="I490" s="6"/>
       <c r="J490" s="6">
@@ -31200,16 +31197,16 @@
       <c r="R490" s="7"/>
       <c r="S490" s="6"/>
       <c r="T490" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U490" s="6"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C491" s="5">
         <v>60</v>
@@ -31227,7 +31224,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31253,18 +31250,18 @@
       <c r="R491" s="7"/>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U491" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="492" spans="1:21">
       <c r="A492" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B492" s="2" t="s">
         <v>999</v>
-      </c>
-      <c r="B492" s="2" t="s">
-        <v>1000</v>
       </c>
       <c r="C492" s="2">
         <v>100</v>
@@ -31282,7 +31279,7 @@
         <v>0</v>
       </c>
       <c r="H492" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I492" s="2"/>
       <c r="J492" s="2">
@@ -31310,16 +31307,16 @@
         <v>4</v>
       </c>
       <c r="T492" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="U492" s="2"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31337,7 +31334,7 @@
         <v>0</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31361,16 +31358,16 @@
       <c r="R493" s="7"/>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31388,7 +31385,7 @@
         <v>1</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31412,16 +31409,16 @@
       <c r="R494" s="7"/>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31439,7 +31436,7 @@
         <v>2</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31463,16 +31460,16 @@
       <c r="R495" s="7"/>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31490,7 +31487,7 @@
         <v>3</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31514,16 +31511,16 @@
       <c r="R496" s="7"/>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U496" s="6"/>
     </row>
     <row r="497" spans="1:21" outlineLevel="1">
       <c r="A497" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B497" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B497" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C497" s="5">
         <v>100</v>
@@ -31541,7 +31538,7 @@
         <v>4</v>
       </c>
       <c r="H497" s="6" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="6"/>
       <c r="J497" s="6">
@@ -31567,16 +31564,16 @@
       <c r="R497" s="7"/>
       <c r="S497" s="6"/>
       <c r="T497" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U497" s="6"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C498" s="5">
         <v>100</v>
@@ -31594,7 +31591,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31620,18 +31617,18 @@
       <c r="R498" s="7"/>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="499" spans="1:21">
       <c r="A499" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B499" s="2" t="s">
         <v>1010</v>
-      </c>
-      <c r="B499" s="2" t="s">
-        <v>1011</v>
       </c>
       <c r="C499" s="2">
         <v>60</v>
@@ -31649,7 +31646,7 @@
         <v>0</v>
       </c>
       <c r="H499" s="2" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I499" s="2"/>
       <c r="J499" s="2">
@@ -31677,16 +31674,16 @@
         <v>5</v>
       </c>
       <c r="T499" s="2" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="U499" s="2"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31704,7 +31701,7 @@
         <v>0</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31728,16 +31725,16 @@
       <c r="R500" s="7"/>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31755,7 +31752,7 @@
         <v>1</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31779,16 +31776,16 @@
       <c r="R501" s="7"/>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31806,7 +31803,7 @@
         <v>2</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31830,16 +31827,16 @@
       <c r="R502" s="7"/>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31857,7 +31854,7 @@
         <v>3</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31881,16 +31878,16 @@
       <c r="R503" s="7"/>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U503" s="6"/>
     </row>
     <row r="504" spans="1:21" outlineLevel="1">
       <c r="A504" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B504" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B504" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C504" s="5">
         <v>60</v>
@@ -31908,7 +31905,7 @@
         <v>4</v>
       </c>
       <c r="H504" s="6" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="6"/>
       <c r="J504" s="6">
@@ -31934,16 +31931,16 @@
       <c r="R504" s="7"/>
       <c r="S504" s="6"/>
       <c r="T504" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U504" s="6"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C505" s="5">
         <v>60</v>
@@ -31961,7 +31958,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31987,18 +31984,18 @@
       <c r="R505" s="7"/>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="506" spans="1:21">
       <c r="A506" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B506" s="2" t="s">
         <v>1021</v>
-      </c>
-      <c r="B506" s="2" t="s">
-        <v>1022</v>
       </c>
       <c r="C506" s="2">
         <v>100</v>
@@ -32016,7 +32013,7 @@
         <v>0</v>
       </c>
       <c r="H506" s="2" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I506" s="2"/>
       <c r="J506" s="2">
@@ -32044,16 +32041,16 @@
         <v>6</v>
       </c>
       <c r="T506" s="2" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="U506" s="2"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32071,7 +32068,7 @@
         <v>0</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32095,16 +32092,16 @@
       <c r="R507" s="7"/>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32122,7 +32119,7 @@
         <v>1</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32146,16 +32143,16 @@
       <c r="R508" s="7"/>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32173,7 +32170,7 @@
         <v>2</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32197,16 +32194,16 @@
       <c r="R509" s="7"/>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32224,7 +32221,7 @@
         <v>3</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32248,16 +32245,16 @@
       <c r="R510" s="7"/>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U510" s="6"/>
     </row>
     <row r="511" spans="1:21" outlineLevel="1">
       <c r="A511" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B511" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B511" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C511" s="5">
         <v>100</v>
@@ -32275,7 +32272,7 @@
         <v>4</v>
       </c>
       <c r="H511" s="6" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I511" s="6"/>
       <c r="J511" s="6">
@@ -32301,16 +32298,16 @@
       <c r="R511" s="7"/>
       <c r="S511" s="6"/>
       <c r="T511" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U511" s="6"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32328,7 +32325,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32354,18 +32351,18 @@
       <c r="R512" s="7"/>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
+        <v>1030</v>
+      </c>
+      <c r="U512" s="6" t="s">
         <v>1031</v>
-      </c>
-      <c r="U512" s="6" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="513" spans="1:21">
       <c r="A513" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B513" s="2" t="s">
         <v>1033</v>
-      </c>
-      <c r="B513" s="2" t="s">
-        <v>1034</v>
       </c>
       <c r="C513" s="2">
         <v>100</v>
@@ -32383,7 +32380,7 @@
         <v>0</v>
       </c>
       <c r="H513" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I513" s="2"/>
       <c r="J513" s="2">
@@ -32411,16 +32408,16 @@
         <v>7</v>
       </c>
       <c r="T513" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="U513" s="2"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32438,7 +32435,7 @@
         <v>0</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32462,16 +32459,16 @@
       <c r="R514" s="7"/>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32489,7 +32486,7 @@
         <v>1</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32513,16 +32510,16 @@
       <c r="R515" s="7"/>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32540,7 +32537,7 @@
         <v>2</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32564,16 +32561,16 @@
       <c r="R516" s="7"/>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32591,7 +32588,7 @@
         <v>3</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32615,16 +32612,16 @@
       <c r="R517" s="7"/>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U517" s="6"/>
     </row>
     <row r="518" spans="1:21" outlineLevel="1">
       <c r="A518" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B518" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B518" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C518" s="5">
         <v>100</v>
@@ -32642,7 +32639,7 @@
         <v>4</v>
       </c>
       <c r="H518" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I518" s="6"/>
       <c r="J518" s="6">
@@ -32668,16 +32665,16 @@
       <c r="R518" s="7"/>
       <c r="S518" s="6"/>
       <c r="T518" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U518" s="6"/>
     </row>
     <row r="519" spans="1:21" outlineLevel="1">
       <c r="A519" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B519" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B519" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C519" s="5">
         <v>100</v>
@@ -32695,7 +32692,7 @@
         <v>0</v>
       </c>
       <c r="H519" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="I519" s="6"/>
       <c r="J519" s="6">
@@ -32721,10 +32718,10 @@
       <c r="R519" s="7"/>
       <c r="S519" s="6"/>
       <c r="T519" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U519" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generated from ./SC24/HVCB.json at e2ff674
</commit_message>
<xml_diff>
--- a/SC24/artifacts/HVCB/HVCB.xlsx
+++ b/SC24/artifacts/HVCB/HVCB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5998" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5998" uniqueCount="1043">
   <si>
     <t>ID</t>
   </si>
@@ -2816,9 +2816,6 @@
   </si>
   <si>
     <t>HVB_stResIsol</t>
-  </si>
-  <si>
-    <t>STOPPED</t>
   </si>
   <si>
     <t>OK</t>
@@ -29242,7 +29239,7 @@
         <v>0</v>
       </c>
       <c r="T453" s="2" t="s">
-        <v>933</v>
+        <v>863</v>
       </c>
       <c r="U453" s="2"/>
     </row>
@@ -29301,7 +29298,7 @@
         <v>1</v>
       </c>
       <c r="T454" s="6" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="U454" s="5"/>
     </row>
@@ -29360,7 +29357,7 @@
         <v>2</v>
       </c>
       <c r="T455" s="6" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="U455" s="5"/>
     </row>
@@ -29419,7 +29416,7 @@
         <v>3</v>
       </c>
       <c r="T456" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="U456" s="5"/>
     </row>
@@ -29478,7 +29475,7 @@
         <v>4</v>
       </c>
       <c r="T457" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="U457" s="5"/>
     </row>
@@ -29537,7 +29534,7 @@
         <v>6</v>
       </c>
       <c r="T458" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="U458" s="5"/>
     </row>
@@ -29564,10 +29561,10 @@
         <v>0</v>
       </c>
       <c r="H459" s="6" t="s">
+        <v>938</v>
+      </c>
+      <c r="I459" s="6" t="s">
         <v>939</v>
-      </c>
-      <c r="I459" s="6" t="s">
-        <v>940</v>
       </c>
       <c r="J459" s="6">
         <v>16</v>
@@ -29594,18 +29591,18 @@
       </c>
       <c r="S459" s="6"/>
       <c r="T459" s="6" t="s">
+        <v>940</v>
+      </c>
+      <c r="U459" s="6" t="s">
         <v>941</v>
-      </c>
-      <c r="U459" s="6" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="460" spans="1:21">
       <c r="A460" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="B460" s="2" t="s">
         <v>943</v>
-      </c>
-      <c r="B460" s="2" t="s">
-        <v>944</v>
       </c>
       <c r="C460" s="2">
         <v>1000</v>
@@ -29623,10 +29620,10 @@
         <v>0</v>
       </c>
       <c r="H460" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="I460" s="2" t="s">
         <v>945</v>
-      </c>
-      <c r="I460" s="2" t="s">
-        <v>946</v>
       </c>
       <c r="J460" s="2">
         <v>32</v>
@@ -29653,16 +29650,16 @@
       </c>
       <c r="S460" s="2"/>
       <c r="T460" s="2" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="U460" s="2"/>
     </row>
     <row r="461" spans="1:21" outlineLevel="1">
       <c r="A461" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="B461" s="5" t="s">
         <v>943</v>
-      </c>
-      <c r="B461" s="5" t="s">
-        <v>944</v>
       </c>
       <c r="C461" s="5">
         <v>1000</v>
@@ -29680,10 +29677,10 @@
         <v>0</v>
       </c>
       <c r="H461" s="6" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="I461" s="6" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="J461" s="6">
         <v>32</v>
@@ -29710,22 +29707,22 @@
       </c>
       <c r="S461" s="6"/>
       <c r="T461" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="U461" s="6"/>
     </row>
     <row r="462" spans="1:21">
       <c r="A462" s="2" t="s">
+        <v>948</v>
+      </c>
+      <c r="B462" s="2" t="s">
         <v>949</v>
       </c>
-      <c r="B462" s="2" t="s">
+      <c r="C462" s="2">
+        <v>0</v>
+      </c>
+      <c r="D462" s="2" t="s">
         <v>950</v>
-      </c>
-      <c r="C462" s="2">
-        <v>0</v>
-      </c>
-      <c r="D462" s="2" t="s">
-        <v>951</v>
       </c>
       <c r="E462" s="2" t="s">
         <v>24</v>
@@ -29751,16 +29748,16 @@
     </row>
     <row r="463" spans="1:21">
       <c r="A463" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="B463" s="2" t="s">
         <v>952</v>
       </c>
-      <c r="B463" s="2" t="s">
+      <c r="C463" s="2">
+        <v>0</v>
+      </c>
+      <c r="D463" s="2" t="s">
         <v>953</v>
-      </c>
-      <c r="C463" s="2">
-        <v>0</v>
-      </c>
-      <c r="D463" s="2" t="s">
-        <v>954</v>
       </c>
       <c r="E463" s="2" t="s">
         <v>24</v>
@@ -29786,10 +29783,10 @@
     </row>
     <row r="464" spans="1:21">
       <c r="A464" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B464" s="2" t="s">
         <v>955</v>
-      </c>
-      <c r="B464" s="2" t="s">
-        <v>956</v>
       </c>
       <c r="C464" s="2">
         <v>20</v>
@@ -29807,7 +29804,7 @@
         <v>0</v>
       </c>
       <c r="H464" s="2" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="I464" s="2"/>
       <c r="J464" s="2">
@@ -29835,16 +29832,16 @@
         <v>0</v>
       </c>
       <c r="T464" s="2" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="U464" s="2"/>
     </row>
     <row r="465" spans="1:21" outlineLevel="1">
       <c r="A465" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B465" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B465" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C465" s="5">
         <v>20</v>
@@ -29862,7 +29859,7 @@
         <v>0</v>
       </c>
       <c r="H465" s="6" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="I465" s="6"/>
       <c r="J465" s="6">
@@ -29886,16 +29883,16 @@
       <c r="R465" s="7"/>
       <c r="S465" s="6"/>
       <c r="T465" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U465" s="6"/>
     </row>
     <row r="466" spans="1:21" outlineLevel="1">
       <c r="A466" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B466" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B466" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C466" s="5">
         <v>20</v>
@@ -29913,7 +29910,7 @@
         <v>1</v>
       </c>
       <c r="H466" s="6" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="I466" s="6"/>
       <c r="J466" s="6">
@@ -29937,16 +29934,16 @@
       <c r="R466" s="7"/>
       <c r="S466" s="6"/>
       <c r="T466" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U466" s="6"/>
     </row>
     <row r="467" spans="1:21" outlineLevel="1">
       <c r="A467" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B467" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B467" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C467" s="5">
         <v>20</v>
@@ -29964,7 +29961,7 @@
         <v>2</v>
       </c>
       <c r="H467" s="6" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I467" s="6"/>
       <c r="J467" s="6">
@@ -29988,16 +29985,16 @@
       <c r="R467" s="7"/>
       <c r="S467" s="6"/>
       <c r="T467" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U467" s="6"/>
     </row>
     <row r="468" spans="1:21" outlineLevel="1">
       <c r="A468" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B468" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B468" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C468" s="5">
         <v>20</v>
@@ -30015,7 +30012,7 @@
         <v>3</v>
       </c>
       <c r="H468" s="6" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="I468" s="6"/>
       <c r="J468" s="6">
@@ -30039,16 +30036,16 @@
       <c r="R468" s="7"/>
       <c r="S468" s="6"/>
       <c r="T468" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U468" s="6"/>
     </row>
     <row r="469" spans="1:21" outlineLevel="1">
       <c r="A469" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B469" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B469" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C469" s="5">
         <v>20</v>
@@ -30066,7 +30063,7 @@
         <v>4</v>
       </c>
       <c r="H469" s="6" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="I469" s="6"/>
       <c r="J469" s="6">
@@ -30092,16 +30089,16 @@
       </c>
       <c r="S469" s="6"/>
       <c r="T469" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U469" s="6"/>
     </row>
     <row r="470" spans="1:21" outlineLevel="1">
       <c r="A470" s="5" t="s">
+        <v>954</v>
+      </c>
+      <c r="B470" s="5" t="s">
         <v>955</v>
-      </c>
-      <c r="B470" s="5" t="s">
-        <v>956</v>
       </c>
       <c r="C470" s="5">
         <v>20</v>
@@ -30119,7 +30116,7 @@
         <v>0</v>
       </c>
       <c r="H470" s="6" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="I470" s="6"/>
       <c r="J470" s="6">
@@ -30145,18 +30142,18 @@
       </c>
       <c r="S470" s="6"/>
       <c r="T470" s="6" t="s">
+        <v>965</v>
+      </c>
+      <c r="U470" s="6" t="s">
         <v>966</v>
-      </c>
-      <c r="U470" s="6" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="471" spans="1:21">
       <c r="A471" s="2" t="s">
+        <v>967</v>
+      </c>
+      <c r="B471" s="2" t="s">
         <v>968</v>
-      </c>
-      <c r="B471" s="2" t="s">
-        <v>969</v>
       </c>
       <c r="C471" s="2">
         <v>60</v>
@@ -30174,7 +30171,7 @@
         <v>0</v>
       </c>
       <c r="H471" s="2" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="I471" s="2"/>
       <c r="J471" s="2">
@@ -30202,16 +30199,16 @@
         <v>1</v>
       </c>
       <c r="T471" s="2" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="U471" s="2"/>
     </row>
     <row r="472" spans="1:21" outlineLevel="1">
       <c r="A472" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B472" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B472" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C472" s="5">
         <v>60</v>
@@ -30229,7 +30226,7 @@
         <v>0</v>
       </c>
       <c r="H472" s="6" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="I472" s="6"/>
       <c r="J472" s="6">
@@ -30253,16 +30250,16 @@
       <c r="R472" s="7"/>
       <c r="S472" s="6"/>
       <c r="T472" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U472" s="6"/>
     </row>
     <row r="473" spans="1:21" outlineLevel="1">
       <c r="A473" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B473" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B473" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C473" s="5">
         <v>60</v>
@@ -30280,7 +30277,7 @@
         <v>1</v>
       </c>
       <c r="H473" s="6" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="I473" s="6"/>
       <c r="J473" s="6">
@@ -30304,16 +30301,16 @@
       <c r="R473" s="7"/>
       <c r="S473" s="6"/>
       <c r="T473" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U473" s="6"/>
     </row>
     <row r="474" spans="1:21" outlineLevel="1">
       <c r="A474" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B474" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B474" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C474" s="5">
         <v>60</v>
@@ -30331,7 +30328,7 @@
         <v>2</v>
       </c>
       <c r="H474" s="6" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="I474" s="6"/>
       <c r="J474" s="6">
@@ -30355,16 +30352,16 @@
       <c r="R474" s="7"/>
       <c r="S474" s="6"/>
       <c r="T474" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U474" s="6"/>
     </row>
     <row r="475" spans="1:21" outlineLevel="1">
       <c r="A475" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B475" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B475" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C475" s="5">
         <v>60</v>
@@ -30382,7 +30379,7 @@
         <v>3</v>
       </c>
       <c r="H475" s="6" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="I475" s="6"/>
       <c r="J475" s="6">
@@ -30406,16 +30403,16 @@
       <c r="R475" s="7"/>
       <c r="S475" s="6"/>
       <c r="T475" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U475" s="6"/>
     </row>
     <row r="476" spans="1:21" outlineLevel="1">
       <c r="A476" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B476" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B476" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C476" s="5">
         <v>60</v>
@@ -30433,7 +30430,7 @@
         <v>4</v>
       </c>
       <c r="H476" s="6" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="I476" s="6"/>
       <c r="J476" s="6">
@@ -30459,16 +30456,16 @@
       </c>
       <c r="S476" s="6"/>
       <c r="T476" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U476" s="6"/>
     </row>
     <row r="477" spans="1:21" outlineLevel="1">
       <c r="A477" s="5" t="s">
+        <v>967</v>
+      </c>
+      <c r="B477" s="5" t="s">
         <v>968</v>
-      </c>
-      <c r="B477" s="5" t="s">
-        <v>969</v>
       </c>
       <c r="C477" s="5">
         <v>60</v>
@@ -30486,7 +30483,7 @@
         <v>0</v>
       </c>
       <c r="H477" s="6" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="I477" s="6"/>
       <c r="J477" s="6">
@@ -30512,18 +30509,18 @@
       </c>
       <c r="S477" s="6"/>
       <c r="T477" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U477" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="478" spans="1:21">
       <c r="A478" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="B478" s="2" t="s">
         <v>979</v>
-      </c>
-      <c r="B478" s="2" t="s">
-        <v>980</v>
       </c>
       <c r="C478" s="2">
         <v>60</v>
@@ -30541,7 +30538,7 @@
         <v>0</v>
       </c>
       <c r="H478" s="2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="I478" s="2"/>
       <c r="J478" s="2">
@@ -30569,16 +30566,16 @@
         <v>2</v>
       </c>
       <c r="T478" s="2" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="U478" s="2"/>
     </row>
     <row r="479" spans="1:21" outlineLevel="1">
       <c r="A479" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B479" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B479" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C479" s="5">
         <v>60</v>
@@ -30596,7 +30593,7 @@
         <v>0</v>
       </c>
       <c r="H479" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I479" s="6"/>
       <c r="J479" s="6">
@@ -30620,16 +30617,16 @@
       <c r="R479" s="7"/>
       <c r="S479" s="6"/>
       <c r="T479" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U479" s="6"/>
     </row>
     <row r="480" spans="1:21" outlineLevel="1">
       <c r="A480" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B480" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B480" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C480" s="5">
         <v>60</v>
@@ -30647,7 +30644,7 @@
         <v>1</v>
       </c>
       <c r="H480" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="I480" s="6"/>
       <c r="J480" s="6">
@@ -30671,16 +30668,16 @@
       <c r="R480" s="7"/>
       <c r="S480" s="6"/>
       <c r="T480" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U480" s="6"/>
     </row>
     <row r="481" spans="1:21" outlineLevel="1">
       <c r="A481" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B481" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B481" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C481" s="5">
         <v>60</v>
@@ -30698,7 +30695,7 @@
         <v>2</v>
       </c>
       <c r="H481" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I481" s="6"/>
       <c r="J481" s="6">
@@ -30722,16 +30719,16 @@
       <c r="R481" s="7"/>
       <c r="S481" s="6"/>
       <c r="T481" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U481" s="6"/>
     </row>
     <row r="482" spans="1:21" outlineLevel="1">
       <c r="A482" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B482" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B482" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C482" s="5">
         <v>60</v>
@@ -30749,7 +30746,7 @@
         <v>3</v>
       </c>
       <c r="H482" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I482" s="6"/>
       <c r="J482" s="6">
@@ -30773,16 +30770,16 @@
       <c r="R482" s="7"/>
       <c r="S482" s="6"/>
       <c r="T482" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U482" s="6"/>
     </row>
     <row r="483" spans="1:21" outlineLevel="1">
       <c r="A483" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B483" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B483" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C483" s="5">
         <v>60</v>
@@ -30800,7 +30797,7 @@
         <v>4</v>
       </c>
       <c r="H483" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="I483" s="6"/>
       <c r="J483" s="6">
@@ -30826,16 +30823,16 @@
       </c>
       <c r="S483" s="6"/>
       <c r="T483" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U483" s="6"/>
     </row>
     <row r="484" spans="1:21" outlineLevel="1">
       <c r="A484" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="B484" s="5" t="s">
         <v>979</v>
-      </c>
-      <c r="B484" s="5" t="s">
-        <v>980</v>
       </c>
       <c r="C484" s="5">
         <v>60</v>
@@ -30853,7 +30850,7 @@
         <v>0</v>
       </c>
       <c r="H484" s="6" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I484" s="6"/>
       <c r="J484" s="6">
@@ -30879,18 +30876,18 @@
       </c>
       <c r="S484" s="6"/>
       <c r="T484" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U484" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="485" spans="1:21">
       <c r="A485" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B485" s="2" t="s">
         <v>989</v>
-      </c>
-      <c r="B485" s="2" t="s">
-        <v>990</v>
       </c>
       <c r="C485" s="2">
         <v>60</v>
@@ -30908,7 +30905,7 @@
         <v>0</v>
       </c>
       <c r="H485" s="2" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I485" s="2"/>
       <c r="J485" s="2">
@@ -30936,16 +30933,16 @@
         <v>3</v>
       </c>
       <c r="T485" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="U485" s="2"/>
     </row>
     <row r="486" spans="1:21" outlineLevel="1">
       <c r="A486" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B486" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B486" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C486" s="5">
         <v>60</v>
@@ -30963,7 +30960,7 @@
         <v>0</v>
       </c>
       <c r="H486" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="I486" s="6"/>
       <c r="J486" s="6">
@@ -30987,16 +30984,16 @@
       <c r="R486" s="7"/>
       <c r="S486" s="6"/>
       <c r="T486" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U486" s="6"/>
     </row>
     <row r="487" spans="1:21" outlineLevel="1">
       <c r="A487" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B487" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B487" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C487" s="5">
         <v>60</v>
@@ -31014,7 +31011,7 @@
         <v>1</v>
       </c>
       <c r="H487" s="6" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="I487" s="6"/>
       <c r="J487" s="6">
@@ -31038,16 +31035,16 @@
       <c r="R487" s="7"/>
       <c r="S487" s="6"/>
       <c r="T487" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U487" s="6"/>
     </row>
     <row r="488" spans="1:21" outlineLevel="1">
       <c r="A488" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B488" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B488" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C488" s="5">
         <v>60</v>
@@ -31065,7 +31062,7 @@
         <v>2</v>
       </c>
       <c r="H488" s="6" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="I488" s="6"/>
       <c r="J488" s="6">
@@ -31089,16 +31086,16 @@
       <c r="R488" s="7"/>
       <c r="S488" s="6"/>
       <c r="T488" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U488" s="6"/>
     </row>
     <row r="489" spans="1:21" outlineLevel="1">
       <c r="A489" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B489" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B489" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C489" s="5">
         <v>60</v>
@@ -31116,7 +31113,7 @@
         <v>3</v>
       </c>
       <c r="H489" s="6" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I489" s="6"/>
       <c r="J489" s="6">
@@ -31140,16 +31137,16 @@
       <c r="R489" s="7"/>
       <c r="S489" s="6"/>
       <c r="T489" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U489" s="6"/>
     </row>
     <row r="490" spans="1:21" outlineLevel="1">
       <c r="A490" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B490" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B490" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C490" s="5">
         <v>60</v>
@@ -31167,7 +31164,7 @@
         <v>4</v>
       </c>
       <c r="H490" s="6" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="I490" s="6"/>
       <c r="J490" s="6">
@@ -31193,16 +31190,16 @@
       </c>
       <c r="S490" s="6"/>
       <c r="T490" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U490" s="6"/>
     </row>
     <row r="491" spans="1:21" outlineLevel="1">
       <c r="A491" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="B491" s="5" t="s">
         <v>989</v>
-      </c>
-      <c r="B491" s="5" t="s">
-        <v>990</v>
       </c>
       <c r="C491" s="5">
         <v>60</v>
@@ -31220,7 +31217,7 @@
         <v>0</v>
       </c>
       <c r="H491" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="I491" s="6"/>
       <c r="J491" s="6">
@@ -31246,18 +31243,18 @@
       </c>
       <c r="S491" s="6"/>
       <c r="T491" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U491" s="6" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="492" spans="1:21">
       <c r="A492" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="B492" s="2" t="s">
         <v>999</v>
-      </c>
-      <c r="B492" s="2" t="s">
-        <v>1000</v>
       </c>
       <c r="C492" s="2">
         <v>100</v>
@@ -31275,7 +31272,7 @@
         <v>0</v>
       </c>
       <c r="H492" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I492" s="2"/>
       <c r="J492" s="2">
@@ -31303,16 +31300,16 @@
         <v>4</v>
       </c>
       <c r="T492" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="U492" s="2"/>
     </row>
     <row r="493" spans="1:21" outlineLevel="1">
       <c r="A493" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B493" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B493" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C493" s="5">
         <v>100</v>
@@ -31330,7 +31327,7 @@
         <v>0</v>
       </c>
       <c r="H493" s="6" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I493" s="6"/>
       <c r="J493" s="6">
@@ -31354,16 +31351,16 @@
       <c r="R493" s="7"/>
       <c r="S493" s="6"/>
       <c r="T493" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U493" s="6"/>
     </row>
     <row r="494" spans="1:21" outlineLevel="1">
       <c r="A494" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B494" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B494" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C494" s="5">
         <v>100</v>
@@ -31381,7 +31378,7 @@
         <v>1</v>
       </c>
       <c r="H494" s="6" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="I494" s="6"/>
       <c r="J494" s="6">
@@ -31405,16 +31402,16 @@
       <c r="R494" s="7"/>
       <c r="S494" s="6"/>
       <c r="T494" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U494" s="6"/>
     </row>
     <row r="495" spans="1:21" outlineLevel="1">
       <c r="A495" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B495" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B495" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C495" s="5">
         <v>100</v>
@@ -31432,7 +31429,7 @@
         <v>2</v>
       </c>
       <c r="H495" s="6" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="I495" s="6"/>
       <c r="J495" s="6">
@@ -31456,16 +31453,16 @@
       <c r="R495" s="7"/>
       <c r="S495" s="6"/>
       <c r="T495" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U495" s="6"/>
     </row>
     <row r="496" spans="1:21" outlineLevel="1">
       <c r="A496" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B496" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B496" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C496" s="5">
         <v>100</v>
@@ -31483,7 +31480,7 @@
         <v>3</v>
       </c>
       <c r="H496" s="6" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="I496" s="6"/>
       <c r="J496" s="6">
@@ -31507,16 +31504,16 @@
       <c r="R496" s="7"/>
       <c r="S496" s="6"/>
       <c r="T496" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U496" s="6"/>
     </row>
     <row r="497" spans="1:21" outlineLevel="1">
       <c r="A497" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B497" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B497" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C497" s="5">
         <v>100</v>
@@ -31534,7 +31531,7 @@
         <v>4</v>
       </c>
       <c r="H497" s="6" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="I497" s="6"/>
       <c r="J497" s="6">
@@ -31560,16 +31557,16 @@
       </c>
       <c r="S497" s="6"/>
       <c r="T497" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U497" s="6"/>
     </row>
     <row r="498" spans="1:21" outlineLevel="1">
       <c r="A498" s="5" t="s">
+        <v>998</v>
+      </c>
+      <c r="B498" s="5" t="s">
         <v>999</v>
-      </c>
-      <c r="B498" s="5" t="s">
-        <v>1000</v>
       </c>
       <c r="C498" s="5">
         <v>100</v>
@@ -31587,7 +31584,7 @@
         <v>0</v>
       </c>
       <c r="H498" s="6" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="I498" s="6"/>
       <c r="J498" s="6">
@@ -31613,18 +31610,18 @@
       </c>
       <c r="S498" s="6"/>
       <c r="T498" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U498" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="499" spans="1:21">
       <c r="A499" s="2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B499" s="2" t="s">
         <v>1010</v>
-      </c>
-      <c r="B499" s="2" t="s">
-        <v>1011</v>
       </c>
       <c r="C499" s="2">
         <v>60</v>
@@ -31642,7 +31639,7 @@
         <v>0</v>
       </c>
       <c r="H499" s="2" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="I499" s="2"/>
       <c r="J499" s="2">
@@ -31670,16 +31667,16 @@
         <v>5</v>
       </c>
       <c r="T499" s="2" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="U499" s="2"/>
     </row>
     <row r="500" spans="1:21" outlineLevel="1">
       <c r="A500" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B500" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B500" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C500" s="5">
         <v>60</v>
@@ -31697,7 +31694,7 @@
         <v>0</v>
       </c>
       <c r="H500" s="6" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I500" s="6"/>
       <c r="J500" s="6">
@@ -31721,16 +31718,16 @@
       <c r="R500" s="7"/>
       <c r="S500" s="6"/>
       <c r="T500" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U500" s="6"/>
     </row>
     <row r="501" spans="1:21" outlineLevel="1">
       <c r="A501" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B501" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B501" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C501" s="5">
         <v>60</v>
@@ -31748,7 +31745,7 @@
         <v>1</v>
       </c>
       <c r="H501" s="6" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="I501" s="6"/>
       <c r="J501" s="6">
@@ -31772,16 +31769,16 @@
       <c r="R501" s="7"/>
       <c r="S501" s="6"/>
       <c r="T501" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U501" s="6"/>
     </row>
     <row r="502" spans="1:21" outlineLevel="1">
       <c r="A502" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B502" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B502" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C502" s="5">
         <v>60</v>
@@ -31799,7 +31796,7 @@
         <v>2</v>
       </c>
       <c r="H502" s="6" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="I502" s="6"/>
       <c r="J502" s="6">
@@ -31823,16 +31820,16 @@
       <c r="R502" s="7"/>
       <c r="S502" s="6"/>
       <c r="T502" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U502" s="6"/>
     </row>
     <row r="503" spans="1:21" outlineLevel="1">
       <c r="A503" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B503" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B503" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C503" s="5">
         <v>60</v>
@@ -31850,7 +31847,7 @@
         <v>3</v>
       </c>
       <c r="H503" s="6" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="I503" s="6"/>
       <c r="J503" s="6">
@@ -31874,16 +31871,16 @@
       <c r="R503" s="7"/>
       <c r="S503" s="6"/>
       <c r="T503" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U503" s="6"/>
     </row>
     <row r="504" spans="1:21" outlineLevel="1">
       <c r="A504" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B504" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B504" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C504" s="5">
         <v>60</v>
@@ -31901,7 +31898,7 @@
         <v>4</v>
       </c>
       <c r="H504" s="6" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="I504" s="6"/>
       <c r="J504" s="6">
@@ -31927,16 +31924,16 @@
       </c>
       <c r="S504" s="6"/>
       <c r="T504" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U504" s="6"/>
     </row>
     <row r="505" spans="1:21" outlineLevel="1">
       <c r="A505" s="5" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B505" s="5" t="s">
         <v>1010</v>
-      </c>
-      <c r="B505" s="5" t="s">
-        <v>1011</v>
       </c>
       <c r="C505" s="5">
         <v>60</v>
@@ -31954,7 +31951,7 @@
         <v>0</v>
       </c>
       <c r="H505" s="6" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="I505" s="6"/>
       <c r="J505" s="6">
@@ -31980,18 +31977,18 @@
       </c>
       <c r="S505" s="6"/>
       <c r="T505" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U505" s="6" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="506" spans="1:21">
       <c r="A506" s="2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B506" s="2" t="s">
         <v>1021</v>
-      </c>
-      <c r="B506" s="2" t="s">
-        <v>1022</v>
       </c>
       <c r="C506" s="2">
         <v>100</v>
@@ -32009,7 +32006,7 @@
         <v>0</v>
       </c>
       <c r="H506" s="2" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I506" s="2"/>
       <c r="J506" s="2">
@@ -32037,16 +32034,16 @@
         <v>6</v>
       </c>
       <c r="T506" s="2" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="U506" s="2"/>
     </row>
     <row r="507" spans="1:21" outlineLevel="1">
       <c r="A507" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B507" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B507" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C507" s="5">
         <v>100</v>
@@ -32064,7 +32061,7 @@
         <v>0</v>
       </c>
       <c r="H507" s="6" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I507" s="6"/>
       <c r="J507" s="6">
@@ -32088,16 +32085,16 @@
       <c r="R507" s="7"/>
       <c r="S507" s="6"/>
       <c r="T507" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U507" s="6"/>
     </row>
     <row r="508" spans="1:21" outlineLevel="1">
       <c r="A508" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B508" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B508" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C508" s="5">
         <v>100</v>
@@ -32115,7 +32112,7 @@
         <v>1</v>
       </c>
       <c r="H508" s="6" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I508" s="6"/>
       <c r="J508" s="6">
@@ -32139,16 +32136,16 @@
       <c r="R508" s="7"/>
       <c r="S508" s="6"/>
       <c r="T508" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U508" s="6"/>
     </row>
     <row r="509" spans="1:21" outlineLevel="1">
       <c r="A509" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B509" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B509" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C509" s="5">
         <v>100</v>
@@ -32166,7 +32163,7 @@
         <v>2</v>
       </c>
       <c r="H509" s="6" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I509" s="6"/>
       <c r="J509" s="6">
@@ -32190,16 +32187,16 @@
       <c r="R509" s="7"/>
       <c r="S509" s="6"/>
       <c r="T509" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U509" s="6"/>
     </row>
     <row r="510" spans="1:21" outlineLevel="1">
       <c r="A510" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B510" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B510" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C510" s="5">
         <v>100</v>
@@ -32217,7 +32214,7 @@
         <v>3</v>
       </c>
       <c r="H510" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I510" s="6"/>
       <c r="J510" s="6">
@@ -32241,16 +32238,16 @@
       <c r="R510" s="7"/>
       <c r="S510" s="6"/>
       <c r="T510" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U510" s="6"/>
     </row>
     <row r="511" spans="1:21" outlineLevel="1">
       <c r="A511" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B511" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B511" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C511" s="5">
         <v>100</v>
@@ -32268,7 +32265,7 @@
         <v>4</v>
       </c>
       <c r="H511" s="6" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I511" s="6"/>
       <c r="J511" s="6">
@@ -32294,16 +32291,16 @@
       </c>
       <c r="S511" s="6"/>
       <c r="T511" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U511" s="6"/>
     </row>
     <row r="512" spans="1:21" outlineLevel="1">
       <c r="A512" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B512" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="B512" s="5" t="s">
-        <v>1022</v>
       </c>
       <c r="C512" s="5">
         <v>100</v>
@@ -32321,7 +32318,7 @@
         <v>0</v>
       </c>
       <c r="H512" s="6" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I512" s="6"/>
       <c r="J512" s="6">
@@ -32347,18 +32344,18 @@
       </c>
       <c r="S512" s="6"/>
       <c r="T512" s="6" t="s">
+        <v>1030</v>
+      </c>
+      <c r="U512" s="6" t="s">
         <v>1031</v>
-      </c>
-      <c r="U512" s="6" t="s">
-        <v>1032</v>
       </c>
     </row>
     <row r="513" spans="1:21">
       <c r="A513" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B513" s="2" t="s">
         <v>1033</v>
-      </c>
-      <c r="B513" s="2" t="s">
-        <v>1034</v>
       </c>
       <c r="C513" s="2">
         <v>100</v>
@@ -32376,7 +32373,7 @@
         <v>0</v>
       </c>
       <c r="H513" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I513" s="2"/>
       <c r="J513" s="2">
@@ -32404,16 +32401,16 @@
         <v>7</v>
       </c>
       <c r="T513" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="U513" s="2"/>
     </row>
     <row r="514" spans="1:21" outlineLevel="1">
       <c r="A514" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B514" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B514" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C514" s="5">
         <v>100</v>
@@ -32431,7 +32428,7 @@
         <v>0</v>
       </c>
       <c r="H514" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I514" s="6"/>
       <c r="J514" s="6">
@@ -32455,16 +32452,16 @@
       <c r="R514" s="7"/>
       <c r="S514" s="6"/>
       <c r="T514" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U514" s="6"/>
     </row>
     <row r="515" spans="1:21" outlineLevel="1">
       <c r="A515" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B515" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B515" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C515" s="5">
         <v>100</v>
@@ -32482,7 +32479,7 @@
         <v>1</v>
       </c>
       <c r="H515" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="I515" s="6"/>
       <c r="J515" s="6">
@@ -32506,16 +32503,16 @@
       <c r="R515" s="7"/>
       <c r="S515" s="6"/>
       <c r="T515" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U515" s="6"/>
     </row>
     <row r="516" spans="1:21" outlineLevel="1">
       <c r="A516" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B516" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B516" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C516" s="5">
         <v>100</v>
@@ -32533,7 +32530,7 @@
         <v>2</v>
       </c>
       <c r="H516" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="I516" s="6"/>
       <c r="J516" s="6">
@@ -32557,16 +32554,16 @@
       <c r="R516" s="7"/>
       <c r="S516" s="6"/>
       <c r="T516" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U516" s="6"/>
     </row>
     <row r="517" spans="1:21" outlineLevel="1">
       <c r="A517" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B517" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B517" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C517" s="5">
         <v>100</v>
@@ -32584,7 +32581,7 @@
         <v>3</v>
       </c>
       <c r="H517" s="6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I517" s="6"/>
       <c r="J517" s="6">
@@ -32608,16 +32605,16 @@
       <c r="R517" s="7"/>
       <c r="S517" s="6"/>
       <c r="T517" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U517" s="6"/>
     </row>
     <row r="518" spans="1:21" outlineLevel="1">
       <c r="A518" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B518" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B518" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C518" s="5">
         <v>100</v>
@@ -32635,7 +32632,7 @@
         <v>4</v>
       </c>
       <c r="H518" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I518" s="6"/>
       <c r="J518" s="6">
@@ -32661,16 +32658,16 @@
       </c>
       <c r="S518" s="6"/>
       <c r="T518" s="6" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="U518" s="6"/>
     </row>
     <row r="519" spans="1:21" outlineLevel="1">
       <c r="A519" s="5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B519" s="5" t="s">
         <v>1033</v>
-      </c>
-      <c r="B519" s="5" t="s">
-        <v>1034</v>
       </c>
       <c r="C519" s="5">
         <v>100</v>
@@ -32688,7 +32685,7 @@
         <v>0</v>
       </c>
       <c r="H519" s="6" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="I519" s="6"/>
       <c r="J519" s="6">
@@ -32714,10 +32711,10 @@
       </c>
       <c r="S519" s="6"/>
       <c r="T519" s="6" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="U519" s="6" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>